<commit_message>
xlsx formatted; html preview added
</commit_message>
<xml_diff>
--- a/xlsx/ke.xlsx
+++ b/xlsx/ke.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Tabellenblatt1" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="CORDIC" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,33 +11,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Solving Kepler's equation</t>
   </si>
   <si>
-    <t>E</t>
+    <t>E:</t>
   </si>
   <si>
-    <t>cos E</t>
+    <t>cos E:</t>
   </si>
   <si>
-    <t>sin E</t>
+    <t>sin E:</t>
   </si>
   <si>
-    <t>M</t>
+    <t>M:</t>
   </si>
   <si>
-    <t>e</t>
+    <t>e:</t>
   </si>
   <si>
     <t>CORDIC (two-sided)</t>
   </si>
   <si>
-    <t>E_n+1 = M+e*sin E_n</t>
+    <t>Fix point</t>
   </si>
   <si>
-    <t>Newton E0=M+0.85e</t>
+    <t>Newton</t>
   </si>
   <si>
     <t>n</t>
@@ -67,22 +67,28 @@
     <t>s_n+1</t>
   </si>
   <si>
-    <t>En -E</t>
+    <t>E_n - E</t>
   </si>
   <si>
     <t>E_n</t>
   </si>
   <si>
-    <t xml:space="preserve">  = E_n + s_n*a_n</t>
+    <t>E_n-1 + s_n*a_n</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve"> = E_n - e*cos E_n</t>
+    <t>E_n - e*cos E_n</t>
   </si>
   <si>
     <t xml:space="preserve"> Mn&lt;M</t>
+  </si>
+  <si>
+    <t>E_n+1 = M+e*sin E_n</t>
+  </si>
+  <si>
+    <t>E_0 = M + 0.85e</t>
   </si>
 </sst>
 </file>
@@ -165,7 +171,7 @@
     <col customWidth="1" min="1" max="1" width="5.43"/>
     <col customWidth="1" min="5" max="5" width="6.0"/>
     <col customWidth="1" min="7" max="7" width="16.0"/>
-    <col customWidth="1" min="9" max="9" width="16.71"/>
+    <col customWidth="1" min="9" max="9" width="14.57"/>
     <col customWidth="1" min="10" max="10" width="6.86"/>
     <col customWidth="1" min="12" max="12" width="5.14"/>
   </cols>
@@ -231,41 +237,18 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
       <c r="L6" s="8"/>
-      <c r="M6" s="7" t="s">
-        <v>19</v>
-      </c>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
@@ -281,245 +264,253 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7">
-      <c r="A7" s="2"/>
-      <c r="F7" s="1" t="s">
+      <c r="A7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="8"/>
+      <c r="M7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2"/>
+      <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2">
+      <c r="M8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
         <v>0.0</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F9" s="1">
         <v>0.0</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G9" s="2">
         <v>1.0</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H9" s="2">
         <v>0.0</v>
       </c>
-      <c r="I8">
-        <f t="shared" ref="I8:I64" si="1">F8-$B$4*H8</f>
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <f t="shared" ref="J8:J64" si="2">IF(I8&lt;$B$3,1,-1)</f>
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <f t="shared" ref="K8:K64" si="3">F8-$B$2</f>
+      <c r="I9">
+        <f t="shared" ref="I9:I65" si="1">F9-$B$4*H9</f>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ref="J9:J65" si="2">IF(I9&lt;$B$3,1,-1)</f>
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ref="K9:K65" si="3">F9-$B$2</f>
         <v>-2</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M9" s="2">
         <v>0.12</v>
       </c>
-      <c r="N8">
+      <c r="N9">
         <f>$B$3+0.85*$B$4</f>
         <v>1.940702573</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="2">
+    <row r="10">
+      <c r="A10" s="2">
         <v>1.0</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
         <f>pi()/2</f>
         <v>1.570796327</v>
       </c>
-      <c r="C9">
-        <f t="shared" ref="C9:C64" si="4">cos(B9)</f>
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <f t="shared" ref="D9:D64" si="5">SIN(B9)</f>
-        <v>1</v>
-      </c>
-      <c r="F9" s="3">
-        <f t="shared" ref="F9:F64" si="6">F8+J8*B9</f>
+      <c r="C10">
+        <f t="shared" ref="C10:C65" si="4">cos(B10)</f>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:D65" si="5">SIN(B10)</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" ref="F10:F65" si="6">F9+J9*B10</f>
         <v>1.570796327</v>
       </c>
-      <c r="G9">
-        <f t="shared" ref="G9:G64" si="7">G8*C9-J8*D9*H8</f>
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <f t="shared" ref="H9:H64" si="8">J8*D9*G8+C9*H8</f>
-        <v>1</v>
-      </c>
-      <c r="I9">
+      <c r="G10">
+        <f t="shared" ref="G10:G65" si="7">G9*C10-J9*D10*H9</f>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ref="H10:H65" si="8">J9*D10*G9+C10*H9</f>
+        <v>1</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="1"/>
         <v>0.5707963268</v>
       </c>
-      <c r="J9">
+      <c r="J10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K9">
+      <c r="K10">
         <f t="shared" si="3"/>
         <v>-0.4292036732</v>
       </c>
-      <c r="M9">
-        <f t="shared" ref="M9:M35" si="9">$B$3+$B$4*sin($M8)</f>
+      <c r="M10">
+        <f t="shared" ref="M10:M36" si="9">$B$3+$B$4*sin($M9)</f>
         <v>1.21041478</v>
       </c>
-      <c r="N9">
-        <f t="shared" ref="N9:N25" si="10">N8-(N8-$B$4*SIN(N8)-$B$3)/(1-$B$4*cos(N8))</f>
+      <c r="N10">
+        <f t="shared" ref="N10:N26" si="10">N9-(N9-$B$4*SIN(N9)-$B$3)/(1-$B$4*cos(N9))</f>
         <v>2.001194346</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="2">
+    <row r="11">
+      <c r="A11" s="2">
         <v>2.0</v>
       </c>
-      <c r="B10">
-        <f t="shared" ref="B10:B64" si="11">B9/2</f>
+      <c r="B11">
+        <f t="shared" ref="B11:B65" si="11">B10/2</f>
         <v>0.7853981634</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <f t="shared" si="4"/>
         <v>0.7071067812</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <f t="shared" si="5"/>
         <v>0.7071067812</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F11" s="3">
         <f t="shared" si="6"/>
         <v>2.35619449</v>
       </c>
-      <c r="G10">
+      <c r="G11">
         <f t="shared" si="7"/>
         <v>-0.7071067812</v>
       </c>
-      <c r="H10">
+      <c r="H11">
         <f t="shared" si="8"/>
         <v>0.7071067812</v>
       </c>
-      <c r="I10">
+      <c r="I11">
         <f t="shared" si="1"/>
         <v>1.649087709</v>
       </c>
-      <c r="J10">
+      <c r="J11">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="K10">
+      <c r="K11">
         <f t="shared" si="3"/>
         <v>0.3561944902</v>
       </c>
-      <c r="M10">
+      <c r="M11">
         <f t="shared" si="9"/>
         <v>2.02646492</v>
       </c>
-      <c r="N10">
+      <c r="N11">
         <f t="shared" si="10"/>
         <v>2.000000457</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="2">
+    <row r="12">
+      <c r="A12" s="2">
         <v>3.0</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <f t="shared" si="11"/>
         <v>0.3926990817</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <f t="shared" si="4"/>
         <v>0.9238795325</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <f t="shared" si="5"/>
         <v>0.3826834324</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F12" s="3">
         <f t="shared" si="6"/>
         <v>1.963495408</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <f t="shared" si="7"/>
         <v>-0.3826834324</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <f t="shared" si="8"/>
         <v>0.9238795325</v>
       </c>
-      <c r="I11">
+      <c r="I12">
         <f t="shared" si="1"/>
         <v>1.039615876</v>
       </c>
-      <c r="J11">
+      <c r="J12">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K11">
+      <c r="K12">
         <f t="shared" si="3"/>
         <v>-0.03650459151</v>
       </c>
-      <c r="M11">
+      <c r="M12">
         <f t="shared" si="9"/>
         <v>1.988669579</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="11"/>
-        <v>0.1963495408</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="4"/>
-        <v>0.9807852804</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="5"/>
-        <v>0.195090322</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" si="6"/>
-        <v>2.159844949</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="7"/>
-        <v>-0.555570233</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="8"/>
-        <v>0.8314696123</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>1.328375337</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="3"/>
-        <v>0.1598449493</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="9"/>
-        <v>2.004656651</v>
       </c>
       <c r="N12">
         <f t="shared" si="10"/>
@@ -528,35 +519,35 @@
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B13">
         <f t="shared" si="11"/>
-        <v>0.09817477042</v>
+        <v>0.1963495408</v>
       </c>
       <c r="C13">
         <f t="shared" si="4"/>
-        <v>0.9951847267</v>
+        <v>0.9807852804</v>
       </c>
       <c r="D13">
         <f t="shared" si="5"/>
-        <v>0.09801714033</v>
+        <v>0.195090322</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="6"/>
-        <v>2.061670179</v>
+        <v>2.159844949</v>
       </c>
       <c r="G13">
         <f t="shared" si="7"/>
-        <v>-0.4713967368</v>
+        <v>-0.555570233</v>
       </c>
       <c r="H13">
         <f t="shared" si="8"/>
-        <v>0.8819212643</v>
+        <v>0.8314696123</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>1.179748915</v>
+        <v>1.328375337</v>
       </c>
       <c r="J13">
         <f t="shared" si="2"/>
@@ -564,11 +555,11 @@
       </c>
       <c r="K13">
         <f t="shared" si="3"/>
-        <v>0.06167017892</v>
+        <v>0.1598449493</v>
       </c>
       <c r="M13">
         <f t="shared" si="9"/>
-        <v>1.998052297</v>
+        <v>2.004656651</v>
       </c>
       <c r="N13">
         <f t="shared" si="10"/>
@@ -577,35 +568,35 @@
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B14">
         <f t="shared" si="11"/>
-        <v>0.04908738521</v>
+        <v>0.09817477042</v>
       </c>
       <c r="C14">
         <f t="shared" si="4"/>
-        <v>0.9987954562</v>
+        <v>0.9951847267</v>
       </c>
       <c r="D14">
         <f t="shared" si="5"/>
-        <v>0.04906767433</v>
+        <v>0.09801714033</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="6"/>
-        <v>2.012582794</v>
+        <v>2.061670179</v>
       </c>
       <c r="G14">
         <f t="shared" si="7"/>
-        <v>-0.4275550934</v>
+        <v>-0.4713967368</v>
       </c>
       <c r="H14">
         <f t="shared" si="8"/>
-        <v>0.9039892931</v>
+        <v>0.8819212643</v>
       </c>
       <c r="I14">
         <f t="shared" si="1"/>
-        <v>1.108593501</v>
+        <v>1.179748915</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
@@ -613,11 +604,11 @@
       </c>
       <c r="K14">
         <f t="shared" si="3"/>
-        <v>0.01258279371</v>
+        <v>0.06167017892</v>
       </c>
       <c r="M14">
         <f t="shared" si="9"/>
-        <v>2.000808805</v>
+        <v>1.998052297</v>
       </c>
       <c r="N14">
         <f t="shared" si="10"/>
@@ -626,47 +617,47 @@
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B15">
         <f t="shared" si="11"/>
-        <v>0.02454369261</v>
+        <v>0.04908738521</v>
       </c>
       <c r="C15">
         <f t="shared" si="4"/>
-        <v>0.9996988187</v>
+        <v>0.9987954562</v>
       </c>
       <c r="D15">
         <f t="shared" si="5"/>
-        <v>0.02454122852</v>
+        <v>0.04906767433</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="6"/>
-        <v>1.988039101</v>
+        <v>2.012582794</v>
       </c>
       <c r="G15">
         <f t="shared" si="7"/>
-        <v>-0.405241314</v>
+        <v>-0.4275550934</v>
       </c>
       <c r="H15">
         <f t="shared" si="8"/>
-        <v>0.9142097557</v>
+        <v>0.9039892931</v>
       </c>
       <c r="I15">
         <f t="shared" si="1"/>
-        <v>1.073829345</v>
+        <v>1.108593501</v>
       </c>
       <c r="J15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K15">
         <f t="shared" si="3"/>
-        <v>-0.0119608989</v>
+        <v>0.01258279371</v>
       </c>
       <c r="M15">
         <f t="shared" si="9"/>
-        <v>1.999663121</v>
+        <v>2.000808805</v>
       </c>
       <c r="N15">
         <f t="shared" si="10"/>
@@ -675,47 +666,47 @@
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B16">
         <f t="shared" si="11"/>
-        <v>0.0122718463</v>
+        <v>0.02454369261</v>
       </c>
       <c r="C16">
         <f t="shared" si="4"/>
-        <v>0.9999247018</v>
+        <v>0.9996988187</v>
       </c>
       <c r="D16">
         <f t="shared" si="5"/>
-        <v>0.01227153829</v>
+        <v>0.02454122852</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="6"/>
-        <v>2.000310947</v>
+        <v>1.988039101</v>
       </c>
       <c r="G16">
         <f t="shared" si="7"/>
-        <v>-0.4164295601</v>
+        <v>-0.405241314</v>
       </c>
       <c r="H16">
         <f t="shared" si="8"/>
-        <v>0.9091679831</v>
+        <v>0.9142097557</v>
       </c>
       <c r="I16">
         <f t="shared" si="1"/>
-        <v>1.091142964</v>
+        <v>1.073829345</v>
       </c>
       <c r="J16">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K16">
         <f t="shared" si="3"/>
-        <v>0.0003109474029</v>
+        <v>-0.0119608989</v>
       </c>
       <c r="M16">
         <f t="shared" si="9"/>
-        <v>2.00014014</v>
+        <v>1.999663121</v>
       </c>
       <c r="N16">
         <f t="shared" si="10"/>
@@ -724,47 +715,47 @@
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B17">
         <f t="shared" si="11"/>
-        <v>0.006135923152</v>
+        <v>0.0122718463</v>
       </c>
       <c r="C17">
         <f t="shared" si="4"/>
-        <v>0.9999811753</v>
+        <v>0.9999247018</v>
       </c>
       <c r="D17">
         <f t="shared" si="5"/>
-        <v>0.006135884649</v>
+        <v>0.01227153829</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="6"/>
-        <v>1.994175024</v>
+        <v>2.000310947</v>
       </c>
       <c r="G17">
         <f t="shared" si="7"/>
-        <v>-0.4108431711</v>
+        <v>-0.4164295601</v>
       </c>
       <c r="H17">
         <f t="shared" si="8"/>
-        <v>0.911706032</v>
+        <v>0.9091679831</v>
       </c>
       <c r="I17">
         <f t="shared" si="1"/>
-        <v>1.082468992</v>
+        <v>1.091142964</v>
       </c>
       <c r="J17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K17">
         <f t="shared" si="3"/>
-        <v>-0.005824975749</v>
+        <v>0.0003109474029</v>
       </c>
       <c r="M17">
         <f t="shared" si="9"/>
-        <v>1.999941672</v>
+        <v>2.00014014</v>
       </c>
       <c r="N17">
         <f t="shared" si="10"/>
@@ -773,35 +764,35 @@
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B18">
         <f t="shared" si="11"/>
-        <v>0.003067961576</v>
+        <v>0.006135923152</v>
       </c>
       <c r="C18">
         <f t="shared" si="4"/>
-        <v>0.9999952938</v>
+        <v>0.9999811753</v>
       </c>
       <c r="D18">
         <f t="shared" si="5"/>
-        <v>0.003067956763</v>
+        <v>0.006135884649</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="6"/>
-        <v>1.997242986</v>
+        <v>1.994175024</v>
       </c>
       <c r="G18">
         <f t="shared" si="7"/>
-        <v>-0.4136383122</v>
+        <v>-0.4108431711</v>
       </c>
       <c r="H18">
         <f t="shared" si="8"/>
-        <v>0.9104412923</v>
+        <v>0.911706032</v>
       </c>
       <c r="I18">
         <f t="shared" si="1"/>
-        <v>1.086801694</v>
+        <v>1.082468992</v>
       </c>
       <c r="J18">
         <f t="shared" si="2"/>
@@ -809,11 +800,11 @@
       </c>
       <c r="K18">
         <f t="shared" si="3"/>
-        <v>-0.002757014173</v>
+        <v>-0.005824975749</v>
       </c>
       <c r="M18">
         <f t="shared" si="9"/>
-        <v>2.000024271</v>
+        <v>1.999941672</v>
       </c>
       <c r="N18">
         <f t="shared" si="10"/>
@@ -822,35 +813,35 @@
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="B19">
         <f t="shared" si="11"/>
-        <v>0.001533980788</v>
+        <v>0.003067961576</v>
       </c>
       <c r="C19">
         <f t="shared" si="4"/>
-        <v>0.9999988235</v>
+        <v>0.9999952938</v>
       </c>
       <c r="D19">
         <f t="shared" si="5"/>
-        <v>0.001533980186</v>
+        <v>0.003067956763</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="6"/>
-        <v>1.998776967</v>
+        <v>1.997242986</v>
       </c>
       <c r="G19">
         <f t="shared" si="7"/>
-        <v>-0.4150344245</v>
+        <v>-0.4136383122</v>
       </c>
       <c r="H19">
         <f t="shared" si="8"/>
-        <v>0.9098057081</v>
+        <v>0.9104412923</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
-        <v>1.088971259</v>
+        <v>1.086801694</v>
       </c>
       <c r="J19">
         <f t="shared" si="2"/>
@@ -858,11 +849,11 @@
       </c>
       <c r="K19">
         <f t="shared" si="3"/>
-        <v>-0.001223033385</v>
+        <v>-0.002757014173</v>
       </c>
       <c r="M19">
         <f t="shared" si="9"/>
-        <v>1.999989899</v>
+        <v>2.000024271</v>
       </c>
       <c r="N19">
         <f t="shared" si="10"/>
@@ -871,35 +862,35 @@
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="B20">
         <f t="shared" si="11"/>
-        <v>0.0007669903939</v>
+        <v>0.001533980788</v>
       </c>
       <c r="C20">
         <f t="shared" si="4"/>
-        <v>0.9999997059</v>
+        <v>0.9999988235</v>
       </c>
       <c r="D20">
         <f t="shared" si="5"/>
-        <v>0.0007669903187</v>
+        <v>0.001533980186</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="6"/>
-        <v>1.999543957</v>
+        <v>1.998776967</v>
       </c>
       <c r="G20">
         <f t="shared" si="7"/>
-        <v>-0.4157321146</v>
+        <v>-0.4150344245</v>
       </c>
       <c r="H20">
         <f t="shared" si="8"/>
-        <v>0.9094871131</v>
+        <v>0.9098057081</v>
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
-        <v>1.090056844</v>
+        <v>1.088971259</v>
       </c>
       <c r="J20">
         <f t="shared" si="2"/>
@@ -907,11 +898,11 @@
       </c>
       <c r="K20">
         <f t="shared" si="3"/>
-        <v>-0.0004560429911</v>
+        <v>-0.001223033385</v>
       </c>
       <c r="M20">
         <f t="shared" si="9"/>
-        <v>2.000004203</v>
+        <v>1.999989899</v>
       </c>
       <c r="N20">
         <f t="shared" si="10"/>
@@ -920,35 +911,35 @@
     </row>
     <row r="21">
       <c r="A21" s="2">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="B21">
         <f t="shared" si="11"/>
-        <v>0.000383495197</v>
+        <v>0.0007669903939</v>
       </c>
       <c r="C21">
         <f t="shared" si="4"/>
-        <v>0.9999999265</v>
+        <v>0.9999997059</v>
       </c>
       <c r="D21">
         <f t="shared" si="5"/>
-        <v>0.0003834951876</v>
+        <v>0.0007669903187</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="6"/>
-        <v>1.999927452</v>
+        <v>1.999543957</v>
       </c>
       <c r="G21">
         <f t="shared" si="7"/>
-        <v>-0.4160808679</v>
+        <v>-0.4157321146</v>
       </c>
       <c r="H21">
         <f t="shared" si="8"/>
-        <v>0.909327615</v>
+        <v>0.9094871131</v>
       </c>
       <c r="I21">
         <f t="shared" si="1"/>
-        <v>1.090599837</v>
+        <v>1.090056844</v>
       </c>
       <c r="J21">
         <f t="shared" si="2"/>
@@ -956,11 +947,11 @@
       </c>
       <c r="K21">
         <f t="shared" si="3"/>
-        <v>-0.0000725477941</v>
+        <v>-0.0004560429911</v>
       </c>
       <c r="M21">
         <f t="shared" si="9"/>
-        <v>1.999998251</v>
+        <v>2.000004203</v>
       </c>
       <c r="N21">
         <f t="shared" si="10"/>
@@ -969,47 +960,47 @@
     </row>
     <row r="22">
       <c r="A22" s="2">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="B22">
         <f t="shared" si="11"/>
-        <v>0.0001917475985</v>
+        <v>0.000383495197</v>
       </c>
       <c r="C22">
         <f t="shared" si="4"/>
-        <v>0.9999999816</v>
+        <v>0.9999999265</v>
       </c>
       <c r="D22">
         <f t="shared" si="5"/>
-        <v>0.0001917475973</v>
+        <v>0.0003834951876</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="6"/>
-        <v>2.0001192</v>
+        <v>1.999927452</v>
       </c>
       <c r="G22">
         <f t="shared" si="7"/>
-        <v>-0.4162552217</v>
+        <v>-0.4160808679</v>
       </c>
       <c r="H22">
         <f t="shared" si="8"/>
-        <v>0.9092478157</v>
+        <v>0.909327615</v>
       </c>
       <c r="I22">
         <f t="shared" si="1"/>
-        <v>1.090871384</v>
+        <v>1.090599837</v>
       </c>
       <c r="J22">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K22">
         <f t="shared" si="3"/>
-        <v>0.0001191998044</v>
+        <v>-0.0000725477941</v>
       </c>
       <c r="M22">
         <f t="shared" si="9"/>
-        <v>2.000000728</v>
+        <v>1.999998251</v>
       </c>
       <c r="N22">
         <f t="shared" si="10"/>
@@ -1018,35 +1009,35 @@
     </row>
     <row r="23">
       <c r="A23" s="2">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="B23">
         <f t="shared" si="11"/>
-        <v>0.00009587379924</v>
+        <v>0.0001917475985</v>
       </c>
       <c r="C23">
         <f t="shared" si="4"/>
-        <v>0.9999999954</v>
+        <v>0.9999999816</v>
       </c>
       <c r="D23">
         <f t="shared" si="5"/>
-        <v>0.0000958737991</v>
+        <v>0.0001917475973</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="6"/>
-        <v>2.000023326</v>
+        <v>2.0001192</v>
       </c>
       <c r="G23">
         <f t="shared" si="7"/>
-        <v>-0.4161680467</v>
+        <v>-0.4162552217</v>
       </c>
       <c r="H23">
         <f t="shared" si="8"/>
-        <v>0.9092877195</v>
+        <v>0.9092478157</v>
       </c>
       <c r="I23">
         <f t="shared" si="1"/>
-        <v>1.090735606</v>
+        <v>1.090871384</v>
       </c>
       <c r="J23">
         <f t="shared" si="2"/>
@@ -1054,11 +1045,11 @@
       </c>
       <c r="K23">
         <f t="shared" si="3"/>
-        <v>0.00002332600515</v>
+        <v>0.0001191998044</v>
       </c>
       <c r="M23">
         <f t="shared" si="9"/>
-        <v>1.999999697</v>
+        <v>2.000000728</v>
       </c>
       <c r="N23">
         <f t="shared" si="10"/>
@@ -1067,47 +1058,47 @@
     </row>
     <row r="24">
       <c r="A24" s="2">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="B24">
         <f t="shared" si="11"/>
-        <v>0.00004793689962</v>
+        <v>0.00009587379924</v>
       </c>
       <c r="C24">
         <f t="shared" si="4"/>
-        <v>0.9999999989</v>
+        <v>0.9999999954</v>
       </c>
       <c r="D24">
         <f t="shared" si="5"/>
-        <v>0.0000479368996</v>
+        <v>0.0000958737991</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="6"/>
-        <v>1.999975389</v>
+        <v>2.000023326</v>
       </c>
       <c r="G24">
         <f t="shared" si="7"/>
-        <v>-0.4161244578</v>
+        <v>-0.4161680467</v>
       </c>
       <c r="H24">
         <f t="shared" si="8"/>
-        <v>0.9093076683</v>
+        <v>0.9092877195</v>
       </c>
       <c r="I24">
         <f t="shared" si="1"/>
-        <v>1.090667721</v>
+        <v>1.090735606</v>
       </c>
       <c r="J24">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K24">
         <f t="shared" si="3"/>
-        <v>-0.00002461089447</v>
+        <v>0.00002332600515</v>
       </c>
       <c r="M24">
         <f t="shared" si="9"/>
-        <v>2.000000126</v>
+        <v>1.999999697</v>
       </c>
       <c r="N24">
         <f t="shared" si="10"/>
@@ -1116,35 +1107,35 @@
     </row>
     <row r="25">
       <c r="A25" s="2">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
       <c r="B25">
         <f t="shared" si="11"/>
-        <v>0.00002396844981</v>
+        <v>0.00004793689962</v>
       </c>
       <c r="C25">
         <f t="shared" si="4"/>
-        <v>0.9999999997</v>
+        <v>0.9999999989</v>
       </c>
       <c r="D25">
         <f t="shared" si="5"/>
-        <v>0.00002396844981</v>
+        <v>0.0000479368996</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="6"/>
-        <v>1.999999358</v>
+        <v>1.999975389</v>
       </c>
       <c r="G25">
         <f t="shared" si="7"/>
-        <v>-0.4161462524</v>
+        <v>-0.4161244578</v>
       </c>
       <c r="H25">
         <f t="shared" si="8"/>
-        <v>0.9092976942</v>
+        <v>0.9093076683</v>
       </c>
       <c r="I25">
         <f t="shared" si="1"/>
-        <v>1.090701663</v>
+        <v>1.090667721</v>
       </c>
       <c r="J25">
         <f t="shared" si="2"/>
@@ -1152,11 +1143,11 @@
       </c>
       <c r="K25">
         <f t="shared" si="3"/>
-        <v>-0.0000006424446628</v>
+        <v>-0.00002461089447</v>
       </c>
       <c r="M25">
         <f t="shared" si="9"/>
-        <v>1.999999948</v>
+        <v>2.000000126</v>
       </c>
       <c r="N25">
         <f t="shared" si="10"/>
@@ -1165,80 +1156,84 @@
     </row>
     <row r="26">
       <c r="A26" s="2">
-        <v>18.0</v>
+        <v>17.0</v>
       </c>
       <c r="B26">
         <f t="shared" si="11"/>
-        <v>0.00001198422491</v>
+        <v>0.00002396844981</v>
       </c>
       <c r="C26">
         <f t="shared" si="4"/>
-        <v>0.9999999999</v>
+        <v>0.9999999997</v>
       </c>
       <c r="D26">
         <f t="shared" si="5"/>
-        <v>0.00001198422491</v>
+        <v>0.00002396844981</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="6"/>
-        <v>2.000011342</v>
+        <v>1.999999358</v>
       </c>
       <c r="G26">
         <f t="shared" si="7"/>
-        <v>-0.4161571496</v>
+        <v>-0.4161462524</v>
       </c>
       <c r="H26">
         <f t="shared" si="8"/>
-        <v>0.9092927069</v>
+        <v>0.9092976942</v>
       </c>
       <c r="I26">
         <f t="shared" si="1"/>
-        <v>1.090718635</v>
+        <v>1.090701663</v>
       </c>
       <c r="J26">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K26">
         <f t="shared" si="3"/>
-        <v>0.00001134178024</v>
+        <v>-0.0000006424446628</v>
       </c>
       <c r="M26">
         <f t="shared" si="9"/>
-        <v>2.000000022</v>
+        <v>1.999999948</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="10"/>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2">
-        <v>19.0</v>
+        <v>18.0</v>
       </c>
       <c r="B27">
         <f t="shared" si="11"/>
-        <v>0.000005992112453</v>
+        <v>0.00001198422491</v>
       </c>
       <c r="C27">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.9999999999</v>
       </c>
       <c r="D27">
         <f t="shared" si="5"/>
-        <v>0.000005992112453</v>
+        <v>0.00001198422491</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="6"/>
-        <v>2.00000535</v>
+        <v>2.000011342</v>
       </c>
       <c r="G27">
         <f t="shared" si="7"/>
-        <v>-0.416151701</v>
+        <v>-0.4161571496</v>
       </c>
       <c r="H27">
         <f t="shared" si="8"/>
-        <v>0.9092952006</v>
+        <v>0.9092927069</v>
       </c>
       <c r="I27">
         <f t="shared" si="1"/>
-        <v>1.090710149</v>
+        <v>1.090718635</v>
       </c>
       <c r="J27">
         <f t="shared" si="2"/>
@@ -1246,20 +1241,20 @@
       </c>
       <c r="K27">
         <f t="shared" si="3"/>
-        <v>0.00000534966779</v>
+        <v>0.00001134178024</v>
       </c>
       <c r="M27">
         <f t="shared" si="9"/>
-        <v>1.999999991</v>
+        <v>2.000000022</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2">
-        <v>20.0</v>
+        <v>19.0</v>
       </c>
       <c r="B28">
         <f t="shared" si="11"/>
-        <v>0.000002996056226</v>
+        <v>0.000005992112453</v>
       </c>
       <c r="C28">
         <f t="shared" si="4"/>
@@ -1267,23 +1262,23 @@
       </c>
       <c r="D28">
         <f t="shared" si="5"/>
-        <v>0.000002996056226</v>
+        <v>0.000005992112453</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="6"/>
-        <v>2.000002354</v>
+        <v>2.00000535</v>
       </c>
       <c r="G28">
         <f t="shared" si="7"/>
-        <v>-0.4161489767</v>
+        <v>-0.416151701</v>
       </c>
       <c r="H28">
         <f t="shared" si="8"/>
-        <v>0.9092964474</v>
+        <v>0.9092952006</v>
       </c>
       <c r="I28">
         <f t="shared" si="1"/>
-        <v>1.090705906</v>
+        <v>1.090710149</v>
       </c>
       <c r="J28">
         <f t="shared" si="2"/>
@@ -1291,20 +1286,20 @@
       </c>
       <c r="K28">
         <f t="shared" si="3"/>
-        <v>0.000002353611563</v>
+        <v>0.00000534966779</v>
       </c>
       <c r="M28">
         <f t="shared" si="9"/>
-        <v>2.000000004</v>
+        <v>1.999999991</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2">
-        <v>21.0</v>
+        <v>20.0</v>
       </c>
       <c r="B29">
         <f t="shared" si="11"/>
-        <v>0.000001498028113</v>
+        <v>0.000002996056226</v>
       </c>
       <c r="C29">
         <f t="shared" si="4"/>
@@ -1312,23 +1307,23 @@
       </c>
       <c r="D29">
         <f t="shared" si="5"/>
-        <v>0.000001498028113</v>
+        <v>0.000002996056226</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="6"/>
-        <v>2.000000856</v>
+        <v>2.000002354</v>
       </c>
       <c r="G29">
         <f t="shared" si="7"/>
-        <v>-0.4161476145</v>
+        <v>-0.4161489767</v>
       </c>
       <c r="H29">
         <f t="shared" si="8"/>
-        <v>0.9092970708</v>
+        <v>0.9092964474</v>
       </c>
       <c r="I29">
         <f t="shared" si="1"/>
-        <v>1.090703785</v>
+        <v>1.090705906</v>
       </c>
       <c r="J29">
         <f t="shared" si="2"/>
@@ -1336,20 +1331,20 @@
       </c>
       <c r="K29">
         <f t="shared" si="3"/>
-        <v>0.0000008555834503</v>
+        <v>0.000002353611563</v>
       </c>
       <c r="M29">
         <f t="shared" si="9"/>
-        <v>1.999999998</v>
+        <v>2.000000004</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2">
-        <v>22.0</v>
+        <v>21.0</v>
       </c>
       <c r="B30">
         <f t="shared" si="11"/>
-        <v>0.0000007490140566</v>
+        <v>0.000001498028113</v>
       </c>
       <c r="C30">
         <f t="shared" si="4"/>
@@ -1357,23 +1352,23 @@
       </c>
       <c r="D30">
         <f t="shared" si="5"/>
-        <v>0.0000007490140566</v>
+        <v>0.000001498028113</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="6"/>
-        <v>2.000000107</v>
+        <v>2.000000856</v>
       </c>
       <c r="G30">
         <f t="shared" si="7"/>
-        <v>-0.4161469335</v>
+        <v>-0.4161476145</v>
       </c>
       <c r="H30">
         <f t="shared" si="8"/>
-        <v>0.9092973825</v>
+        <v>0.9092970708</v>
       </c>
       <c r="I30">
         <f t="shared" si="1"/>
-        <v>1.090702724</v>
+        <v>1.090703785</v>
       </c>
       <c r="J30">
         <f t="shared" si="2"/>
@@ -1381,20 +1376,20 @@
       </c>
       <c r="K30">
         <f t="shared" si="3"/>
-        <v>0.0000001065693938</v>
+        <v>0.0000008555834503</v>
       </c>
       <c r="M30">
         <f t="shared" si="9"/>
-        <v>2.000000001</v>
+        <v>1.999999998</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2">
-        <v>23.0</v>
+        <v>22.0</v>
       </c>
       <c r="B31">
         <f t="shared" si="11"/>
-        <v>0.0000003745070283</v>
+        <v>0.0000007490140566</v>
       </c>
       <c r="C31">
         <f t="shared" si="4"/>
@@ -1402,44 +1397,44 @@
       </c>
       <c r="D31">
         <f t="shared" si="5"/>
-        <v>0.0000003745070283</v>
+        <v>0.0000007490140566</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="6"/>
-        <v>1.999999732</v>
+        <v>2.000000107</v>
       </c>
       <c r="G31">
         <f t="shared" si="7"/>
-        <v>-0.4161465929</v>
+        <v>-0.4161469335</v>
       </c>
       <c r="H31">
         <f t="shared" si="8"/>
-        <v>0.9092975383</v>
+        <v>0.9092973825</v>
       </c>
       <c r="I31">
         <f t="shared" si="1"/>
-        <v>1.090702194</v>
+        <v>1.090702724</v>
       </c>
       <c r="J31">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K31">
         <f t="shared" si="3"/>
-        <v>-0.0000002679376345</v>
+        <v>0.0000001065693938</v>
       </c>
       <c r="M31">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>2.000000001</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2">
-        <v>24.0</v>
+        <v>23.0</v>
       </c>
       <c r="B32">
         <f t="shared" si="11"/>
-        <v>0.0000001872535141</v>
+        <v>0.0000003745070283</v>
       </c>
       <c r="C32">
         <f t="shared" si="4"/>
@@ -1447,23 +1442,23 @@
       </c>
       <c r="D32">
         <f t="shared" si="5"/>
-        <v>0.0000001872535141</v>
+        <v>0.0000003745070283</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" si="6"/>
-        <v>1.999999919</v>
+        <v>1.999999732</v>
       </c>
       <c r="G32">
         <f t="shared" si="7"/>
-        <v>-0.4161467632</v>
+        <v>-0.4161465929</v>
       </c>
       <c r="H32">
         <f t="shared" si="8"/>
-        <v>0.9092974604</v>
+        <v>0.9092975383</v>
       </c>
       <c r="I32">
         <f t="shared" si="1"/>
-        <v>1.090702459</v>
+        <v>1.090702194</v>
       </c>
       <c r="J32">
         <f t="shared" si="2"/>
@@ -1471,7 +1466,7 @@
       </c>
       <c r="K32">
         <f t="shared" si="3"/>
-        <v>-0.00000008068412027</v>
+        <v>-0.0000002679376345</v>
       </c>
       <c r="M32">
         <f t="shared" si="9"/>
@@ -1480,11 +1475,11 @@
     </row>
     <row r="33">
       <c r="A33" s="2">
-        <v>25.0</v>
+        <v>24.0</v>
       </c>
       <c r="B33">
         <f t="shared" si="11"/>
-        <v>0.00000009362675707</v>
+        <v>0.0000001872535141</v>
       </c>
       <c r="C33">
         <f t="shared" si="4"/>
@@ -1492,31 +1487,31 @@
       </c>
       <c r="D33">
         <f t="shared" si="5"/>
-        <v>0.00000009362675707</v>
+        <v>0.0000001872535141</v>
       </c>
       <c r="F33" s="3">
         <f t="shared" si="6"/>
-        <v>2.000000013</v>
+        <v>1.999999919</v>
       </c>
       <c r="G33">
         <f t="shared" si="7"/>
-        <v>-0.4161468483</v>
+        <v>-0.4161467632</v>
       </c>
       <c r="H33">
         <f t="shared" si="8"/>
-        <v>0.9092974214</v>
+        <v>0.9092974604</v>
       </c>
       <c r="I33">
         <f t="shared" si="1"/>
-        <v>1.090702592</v>
+        <v>1.090702459</v>
       </c>
       <c r="J33">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K33">
         <f t="shared" si="3"/>
-        <v>0.00000001294263674</v>
+        <v>-0.00000008068412027</v>
       </c>
       <c r="M33">
         <f t="shared" si="9"/>
@@ -1525,11 +1520,11 @@
     </row>
     <row r="34">
       <c r="A34" s="2">
-        <v>26.0</v>
+        <v>25.0</v>
       </c>
       <c r="B34">
         <f t="shared" si="11"/>
-        <v>0.00000004681337854</v>
+        <v>0.00000009362675707</v>
       </c>
       <c r="C34">
         <f t="shared" si="4"/>
@@ -1537,31 +1532,31 @@
       </c>
       <c r="D34">
         <f t="shared" si="5"/>
-        <v>0.00000004681337854</v>
+        <v>0.00000009362675707</v>
       </c>
       <c r="F34" s="3">
         <f t="shared" si="6"/>
-        <v>1.999999966</v>
+        <v>2.000000013</v>
       </c>
       <c r="G34">
         <f t="shared" si="7"/>
-        <v>-0.4161468057</v>
+        <v>-0.4161468483</v>
       </c>
       <c r="H34">
         <f t="shared" si="8"/>
-        <v>0.9092974409</v>
+        <v>0.9092974214</v>
       </c>
       <c r="I34">
         <f t="shared" si="1"/>
-        <v>1.090702525</v>
+        <v>1.090702592</v>
       </c>
       <c r="J34">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K34">
         <f t="shared" si="3"/>
-        <v>-0.00000003387074177</v>
+        <v>0.00000001294263674</v>
       </c>
       <c r="M34">
         <f t="shared" si="9"/>
@@ -1570,11 +1565,11 @@
     </row>
     <row r="35">
       <c r="A35" s="2">
-        <v>27.0</v>
+        <v>26.0</v>
       </c>
       <c r="B35">
         <f t="shared" si="11"/>
-        <v>0.00000002340668927</v>
+        <v>0.00000004681337854</v>
       </c>
       <c r="C35">
         <f t="shared" si="4"/>
@@ -1582,23 +1577,23 @@
       </c>
       <c r="D35">
         <f t="shared" si="5"/>
-        <v>0.00000002340668927</v>
+        <v>0.00000004681337854</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="6"/>
-        <v>1.99999999</v>
+        <v>1.999999966</v>
       </c>
       <c r="G35">
         <f t="shared" si="7"/>
-        <v>-0.416146827</v>
+        <v>-0.4161468057</v>
       </c>
       <c r="H35">
         <f t="shared" si="8"/>
-        <v>0.9092974312</v>
+        <v>0.9092974409</v>
       </c>
       <c r="I35">
         <f t="shared" si="1"/>
-        <v>1.090702558</v>
+        <v>1.090702525</v>
       </c>
       <c r="J35">
         <f t="shared" si="2"/>
@@ -1606,7 +1601,7 @@
       </c>
       <c r="K35">
         <f t="shared" si="3"/>
-        <v>-0.00000001046405251</v>
+        <v>-0.00000003387074177</v>
       </c>
       <c r="M35">
         <f t="shared" si="9"/>
@@ -1615,11 +1610,11 @@
     </row>
     <row r="36">
       <c r="A36" s="2">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
       <c r="B36">
         <f t="shared" si="11"/>
-        <v>0.00000001170334463</v>
+        <v>0.00000002340668927</v>
       </c>
       <c r="C36">
         <f t="shared" si="4"/>
@@ -1627,40 +1622,44 @@
       </c>
       <c r="D36">
         <f t="shared" si="5"/>
-        <v>0.00000001170334463</v>
+        <v>0.00000002340668927</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="6"/>
-        <v>2.000000001</v>
+        <v>1.99999999</v>
       </c>
       <c r="G36">
         <f t="shared" si="7"/>
-        <v>-0.4161468377</v>
+        <v>-0.416146827</v>
       </c>
       <c r="H36">
         <f t="shared" si="8"/>
-        <v>0.9092974263</v>
+        <v>0.9092974312</v>
       </c>
       <c r="I36">
         <f t="shared" si="1"/>
-        <v>1.090702575</v>
+        <v>1.090702558</v>
       </c>
       <c r="J36">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K36">
         <f t="shared" si="3"/>
-        <v>0.000000001239292224</v>
+        <v>-0.00000001046405251</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="9"/>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2">
-        <v>29.0</v>
+        <v>28.0</v>
       </c>
       <c r="B37">
         <f t="shared" si="11"/>
-        <v>0.000000005851672317</v>
+        <v>0.00000001170334463</v>
       </c>
       <c r="C37">
         <f t="shared" si="4"/>
@@ -1668,40 +1667,40 @@
       </c>
       <c r="D37">
         <f t="shared" si="5"/>
-        <v>0.000000005851672317</v>
+        <v>0.00000001170334463</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" si="6"/>
-        <v>1.999999995</v>
+        <v>2.000000001</v>
       </c>
       <c r="G37">
         <f t="shared" si="7"/>
-        <v>-0.4161468324</v>
+        <v>-0.4161468377</v>
       </c>
       <c r="H37">
         <f t="shared" si="8"/>
-        <v>0.9092974287</v>
+        <v>0.9092974263</v>
       </c>
       <c r="I37">
         <f t="shared" si="1"/>
-        <v>1.090702567</v>
+        <v>1.090702575</v>
       </c>
       <c r="J37">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K37">
         <f t="shared" si="3"/>
-        <v>-0.000000004612380033</v>
+        <v>0.000000001239292224</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2">
-        <v>30.0</v>
+        <v>29.0</v>
       </c>
       <c r="B38">
         <f t="shared" si="11"/>
-        <v>0.000000002925836159</v>
+        <v>0.000000005851672317</v>
       </c>
       <c r="C38">
         <f t="shared" si="4"/>
@@ -1709,23 +1708,23 @@
       </c>
       <c r="D38">
         <f t="shared" si="5"/>
-        <v>0.000000002925836159</v>
+        <v>0.000000005851672317</v>
       </c>
       <c r="F38" s="3">
         <f t="shared" si="6"/>
-        <v>1.999999998</v>
+        <v>1.999999995</v>
       </c>
       <c r="G38">
         <f t="shared" si="7"/>
-        <v>-0.416146835</v>
+        <v>-0.4161468324</v>
       </c>
       <c r="H38">
         <f t="shared" si="8"/>
-        <v>0.9092974275</v>
+        <v>0.9092974287</v>
       </c>
       <c r="I38">
         <f t="shared" si="1"/>
-        <v>1.090702571</v>
+        <v>1.090702567</v>
       </c>
       <c r="J38">
         <f t="shared" si="2"/>
@@ -1733,16 +1732,16 @@
       </c>
       <c r="K38">
         <f t="shared" si="3"/>
-        <v>-0.000000001686543794</v>
+        <v>-0.000000004612380033</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2">
-        <v>31.0</v>
+        <v>30.0</v>
       </c>
       <c r="B39">
         <f t="shared" si="11"/>
-        <v>0.000000001462918079</v>
+        <v>0.000000002925836159</v>
       </c>
       <c r="C39">
         <f t="shared" si="4"/>
@@ -1750,23 +1749,23 @@
       </c>
       <c r="D39">
         <f t="shared" si="5"/>
-        <v>0.000000001462918079</v>
+        <v>0.000000002925836159</v>
       </c>
       <c r="F39" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1.999999998</v>
       </c>
       <c r="G39">
         <f t="shared" si="7"/>
-        <v>-0.4161468363</v>
+        <v>-0.416146835</v>
       </c>
       <c r="H39">
         <f t="shared" si="8"/>
-        <v>0.9092974269</v>
+        <v>0.9092974275</v>
       </c>
       <c r="I39">
         <f t="shared" si="1"/>
-        <v>1.090702573</v>
+        <v>1.090702571</v>
       </c>
       <c r="J39">
         <f t="shared" si="2"/>
@@ -1774,16 +1773,16 @@
       </c>
       <c r="K39">
         <f t="shared" si="3"/>
-        <v>-0.0000000002236257846</v>
+        <v>-0.000000001686543794</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2">
-        <v>32.0</v>
+        <v>31.0</v>
       </c>
       <c r="B40">
         <f t="shared" si="11"/>
-        <v>0.0000000007314590396</v>
+        <v>0.000000001462918079</v>
       </c>
       <c r="C40">
         <f t="shared" si="4"/>
@@ -1791,40 +1790,40 @@
       </c>
       <c r="D40">
         <f t="shared" si="5"/>
-        <v>0.0000000007314590396</v>
+        <v>0.000000001462918079</v>
       </c>
       <c r="F40" s="3">
         <f t="shared" si="6"/>
-        <v>2.000000001</v>
+        <v>2</v>
       </c>
       <c r="G40">
         <f t="shared" si="7"/>
-        <v>-0.416146837</v>
+        <v>-0.4161468363</v>
       </c>
       <c r="H40">
         <f t="shared" si="8"/>
-        <v>0.9092974266</v>
+        <v>0.9092974269</v>
       </c>
       <c r="I40">
         <f t="shared" si="1"/>
-        <v>1.090702574</v>
+        <v>1.090702573</v>
       </c>
       <c r="J40">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K40">
         <f t="shared" si="3"/>
-        <v>0.0000000005078333309</v>
+        <v>-0.0000000002236257846</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2">
-        <v>33.0</v>
+        <v>32.0</v>
       </c>
       <c r="B41">
         <f t="shared" si="11"/>
-        <v>0.0000000003657295198</v>
+        <v>0.0000000007314590396</v>
       </c>
       <c r="C41">
         <f t="shared" si="4"/>
@@ -1832,23 +1831,23 @@
       </c>
       <c r="D41">
         <f t="shared" si="5"/>
-        <v>0.0000000003657295198</v>
+        <v>0.0000000007314590396</v>
       </c>
       <c r="F41" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>2.000000001</v>
       </c>
       <c r="G41">
         <f t="shared" si="7"/>
-        <v>-0.4161468367</v>
+        <v>-0.416146837</v>
       </c>
       <c r="H41">
         <f t="shared" si="8"/>
-        <v>0.9092974268</v>
+        <v>0.9092974266</v>
       </c>
       <c r="I41">
         <f t="shared" si="1"/>
-        <v>1.090702573</v>
+        <v>1.090702574</v>
       </c>
       <c r="J41">
         <f t="shared" si="2"/>
@@ -1856,16 +1855,16 @@
       </c>
       <c r="K41">
         <f t="shared" si="3"/>
-        <v>0.0000000001421036622</v>
+        <v>0.0000000005078333309</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2">
-        <v>34.0</v>
+        <v>33.0</v>
       </c>
       <c r="B42">
         <f t="shared" si="11"/>
-        <v>0.0000000001828647599</v>
+        <v>0.0000000003657295198</v>
       </c>
       <c r="C42">
         <f t="shared" si="4"/>
@@ -1873,7 +1872,7 @@
       </c>
       <c r="D42">
         <f t="shared" si="5"/>
-        <v>0.0000000001828647599</v>
+        <v>0.0000000003657295198</v>
       </c>
       <c r="F42" s="3">
         <f t="shared" si="6"/>
@@ -1881,7 +1880,7 @@
       </c>
       <c r="G42">
         <f t="shared" si="7"/>
-        <v>-0.4161468365</v>
+        <v>-0.4161468367</v>
       </c>
       <c r="H42">
         <f t="shared" si="8"/>
@@ -1893,20 +1892,20 @@
       </c>
       <c r="J42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K42">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.0000000001421036622</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2">
-        <v>35.0</v>
+        <v>34.0</v>
       </c>
       <c r="B43">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.0000000001828647599</v>
       </c>
       <c r="C43">
         <f t="shared" si="4"/>
@@ -1914,7 +1913,7 @@
       </c>
       <c r="D43">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.0000000001828647599</v>
       </c>
       <c r="F43" s="3">
         <f t="shared" si="6"/>
@@ -1922,7 +1921,7 @@
       </c>
       <c r="G43">
         <f t="shared" si="7"/>
-        <v>-0.4161468366</v>
+        <v>-0.4161468365</v>
       </c>
       <c r="H43">
         <f t="shared" si="8"/>
@@ -1934,7 +1933,7 @@
       </c>
       <c r="J43">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K43">
         <f t="shared" si="3"/>
@@ -1943,7 +1942,7 @@
     </row>
     <row r="44">
       <c r="A44" s="2">
-        <v>36.0</v>
+        <v>35.0</v>
       </c>
       <c r="B44">
         <f t="shared" si="11"/>
@@ -1984,7 +1983,7 @@
     </row>
     <row r="45">
       <c r="A45" s="2">
-        <v>37.0</v>
+        <v>36.0</v>
       </c>
       <c r="B45">
         <f t="shared" si="11"/>
@@ -2004,7 +2003,7 @@
       </c>
       <c r="G45">
         <f t="shared" si="7"/>
-        <v>-0.4161468365</v>
+        <v>-0.4161468366</v>
       </c>
       <c r="H45">
         <f t="shared" si="8"/>
@@ -2016,7 +2015,7 @@
       </c>
       <c r="J45">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K45">
         <f t="shared" si="3"/>
@@ -2025,7 +2024,7 @@
     </row>
     <row r="46">
       <c r="A46" s="2">
-        <v>38.0</v>
+        <v>37.0</v>
       </c>
       <c r="B46">
         <f t="shared" si="11"/>
@@ -2066,7 +2065,7 @@
     </row>
     <row r="47">
       <c r="A47" s="2">
-        <v>39.0</v>
+        <v>38.0</v>
       </c>
       <c r="B47">
         <f t="shared" si="11"/>
@@ -2107,7 +2106,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2">
-        <v>40.0</v>
+        <v>39.0</v>
       </c>
       <c r="B48">
         <f t="shared" si="11"/>
@@ -2139,7 +2138,7 @@
       </c>
       <c r="J48">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K48">
         <f t="shared" si="3"/>
@@ -2148,7 +2147,7 @@
     </row>
     <row r="49">
       <c r="A49" s="2">
-        <v>41.0</v>
+        <v>40.0</v>
       </c>
       <c r="B49">
         <f t="shared" si="11"/>
@@ -2189,7 +2188,7 @@
     </row>
     <row r="50">
       <c r="A50" s="2">
-        <v>42.0</v>
+        <v>41.0</v>
       </c>
       <c r="B50">
         <f t="shared" si="11"/>
@@ -2221,7 +2220,7 @@
       </c>
       <c r="J50">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K50">
         <f t="shared" si="3"/>
@@ -2230,7 +2229,7 @@
     </row>
     <row r="51">
       <c r="A51" s="2">
-        <v>43.0</v>
+        <v>42.0</v>
       </c>
       <c r="B51">
         <f t="shared" si="11"/>
@@ -2262,7 +2261,7 @@
       </c>
       <c r="J51">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K51">
         <f t="shared" si="3"/>
@@ -2271,7 +2270,7 @@
     </row>
     <row r="52">
       <c r="A52" s="2">
-        <v>44.0</v>
+        <v>43.0</v>
       </c>
       <c r="B52">
         <f t="shared" si="11"/>
@@ -2312,7 +2311,7 @@
     </row>
     <row r="53">
       <c r="A53" s="2">
-        <v>45.0</v>
+        <v>44.0</v>
       </c>
       <c r="B53">
         <f t="shared" si="11"/>
@@ -2353,7 +2352,7 @@
     </row>
     <row r="54">
       <c r="A54" s="2">
-        <v>46.0</v>
+        <v>45.0</v>
       </c>
       <c r="B54">
         <f t="shared" si="11"/>
@@ -2394,7 +2393,7 @@
     </row>
     <row r="55">
       <c r="A55" s="2">
-        <v>47.0</v>
+        <v>46.0</v>
       </c>
       <c r="B55">
         <f t="shared" si="11"/>
@@ -2426,7 +2425,7 @@
       </c>
       <c r="J55">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K55">
         <f t="shared" si="3"/>
@@ -2435,7 +2434,7 @@
     </row>
     <row r="56">
       <c r="A56" s="2">
-        <v>48.0</v>
+        <v>47.0</v>
       </c>
       <c r="B56">
         <f t="shared" si="11"/>
@@ -2476,7 +2475,7 @@
     </row>
     <row r="57">
       <c r="A57" s="2">
-        <v>49.0</v>
+        <v>48.0</v>
       </c>
       <c r="B57">
         <f t="shared" si="11"/>
@@ -2517,7 +2516,7 @@
     </row>
     <row r="58">
       <c r="A58" s="2">
-        <v>50.0</v>
+        <v>49.0</v>
       </c>
       <c r="B58">
         <f t="shared" si="11"/>
@@ -2558,7 +2557,7 @@
     </row>
     <row r="59">
       <c r="A59" s="2">
-        <v>51.0</v>
+        <v>50.0</v>
       </c>
       <c r="B59">
         <f t="shared" si="11"/>
@@ -2590,7 +2589,7 @@
       </c>
       <c r="J59">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K59">
         <f t="shared" si="3"/>
@@ -2599,7 +2598,7 @@
     </row>
     <row r="60">
       <c r="A60" s="2">
-        <v>52.0</v>
+        <v>51.0</v>
       </c>
       <c r="B60">
         <f t="shared" si="11"/>
@@ -2631,7 +2630,7 @@
       </c>
       <c r="J60">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K60">
         <f t="shared" si="3"/>
@@ -2640,7 +2639,7 @@
     </row>
     <row r="61">
       <c r="A61" s="2">
-        <v>53.0</v>
+        <v>52.0</v>
       </c>
       <c r="B61">
         <f t="shared" si="11"/>
@@ -2672,7 +2671,7 @@
       </c>
       <c r="J61">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K61">
         <f t="shared" si="3"/>
@@ -2681,7 +2680,7 @@
     </row>
     <row r="62">
       <c r="A62" s="2">
-        <v>54.0</v>
+        <v>53.0</v>
       </c>
       <c r="B62">
         <f t="shared" si="11"/>
@@ -2713,7 +2712,7 @@
       </c>
       <c r="J62">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K62">
         <f t="shared" si="3"/>
@@ -2722,7 +2721,7 @@
     </row>
     <row r="63">
       <c r="A63" s="2">
-        <v>55.0</v>
+        <v>54.0</v>
       </c>
       <c r="B63">
         <f t="shared" si="11"/>
@@ -2763,7 +2762,7 @@
     </row>
     <row r="64">
       <c r="A64" s="2">
-        <v>56.0</v>
+        <v>55.0</v>
       </c>
       <c r="B64">
         <f t="shared" si="11"/>
@@ -2803,7 +2802,45 @@
       </c>
     </row>
     <row r="65">
-      <c r="F65" s="3"/>
+      <c r="A65" s="2">
+        <v>56.0</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="7"/>
+        <v>-0.4161468365</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="8"/>
+        <v>0.9092974268</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="1"/>
+        <v>1.090702573</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="F66" s="3"/>
@@ -5615,6 +5652,9 @@
     </row>
     <row r="1002">
       <c r="F1002" s="3"/>
+    </row>
+    <row r="1003">
+      <c r="F1003" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Compatible with online viewer. Fixes #1.
</commit_message>
<xml_diff>
--- a/xlsx/ke.xlsx
+++ b/xlsx/ke.xlsx
@@ -14,9 +14,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
-    <t>Solving Kepler's equation (hyperbolic case) M = e sinh E - E</t>
-  </si>
-  <si>
     <t>Solving Kepler's equation M = E - e sinE</t>
   </si>
   <si>
@@ -26,22 +23,13 @@
     <t>cos E:</t>
   </si>
   <si>
-    <t>cosh E:</t>
-  </si>
-  <si>
     <t>sin E:</t>
-  </si>
-  <si>
-    <t>sinh E:</t>
   </si>
   <si>
     <t>M:</t>
   </si>
   <si>
     <t>e:</t>
-  </si>
-  <si>
-    <t>e*exp(E)/2:</t>
   </si>
   <si>
     <t>CORDIC (two-sided)</t>
@@ -59,19 +47,10 @@
     <t>a_n</t>
   </si>
   <si>
-    <t>cosh a_n</t>
-  </si>
-  <si>
     <t>cos a_n</t>
   </si>
   <si>
-    <t>sinh a_n</t>
-  </si>
-  <si>
     <t>sin a_n</t>
-  </si>
-  <si>
-    <t>m</t>
   </si>
   <si>
     <t>En</t>
@@ -80,13 +59,7 @@
     <t>cos E_n</t>
   </si>
   <si>
-    <t>cosh E_n</t>
-  </si>
-  <si>
     <t>sin E_n</t>
-  </si>
-  <si>
-    <t>sinh E_n</t>
   </si>
   <si>
     <t>M_n</t>
@@ -107,25 +80,52 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>e*sinh E_n - E_n</t>
-  </si>
-  <si>
     <t>E_n - e*sin E_n</t>
   </si>
   <si>
     <t xml:space="preserve"> Mn&lt;M</t>
   </si>
   <si>
+    <t>E_n+1 = M+e*sin E_n</t>
+  </si>
+  <si>
+    <t>E_0 = M + 0.85e</t>
+  </si>
+  <si>
+    <t>Solving Kepler's equation (hyperbolic case) M = e sinh E - E</t>
+  </si>
+  <si>
+    <t>cosh E:</t>
+  </si>
+  <si>
+    <t>sinh E:</t>
+  </si>
+  <si>
+    <t>e*exp(E)/2:</t>
+  </si>
+  <si>
+    <t>cosh a_n</t>
+  </si>
+  <si>
+    <t>sinh a_n</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>cosh E_n</t>
+  </si>
+  <si>
+    <t>sinh E_n</t>
+  </si>
+  <si>
+    <t>e*sinh E_n - E_n</t>
+  </si>
+  <si>
     <t>E_n+1 = e*sinh E_n - M</t>
   </si>
   <si>
-    <t>E_n+1 = M+e*sin E_n</t>
-  </si>
-  <si>
     <t>E_0 = log(abs(M/e) + 1.8)</t>
-  </si>
-  <si>
-    <t>E_0 = M + 0.85e</t>
   </si>
 </sst>
 </file>
@@ -194,10 +194,10 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -248,7 +248,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -256,20 +256,20 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>2.0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2">
         <f>cos(B2)</f>
         <v>-0.4161468365</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2">
         <f>sin(B2)</f>
@@ -278,7 +278,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="6">
         <f>B2-B4*sin(B2)</f>
@@ -288,7 +288,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5">
         <v>1.0</v>
@@ -297,13 +297,13 @@
     </row>
     <row r="5">
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -312,7 +312,7 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="10"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -335,42 +335,42 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="H7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="J7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
@@ -388,23 +388,23 @@
     <row r="8">
       <c r="A8" s="2"/>
       <c r="F8" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -5756,7 +5756,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -5764,48 +5764,48 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2">
         <f> COSH(B2)</f>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="F2">
         <f> SINH(B2)</f>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="6">
         <f> B4*SINH(B2) - B2</f>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <f> exp(B2)/2*B4</f>
-        <v>3.694528049</v>
+        <v>74.20657955</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="9"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5">
         <v>1.0</v>
@@ -5815,13 +5815,13 @@
     </row>
     <row r="5">
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -5830,7 +5830,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="10"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -5853,44 +5853,44 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="G7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="K7" s="7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
@@ -5908,21 +5908,21 @@
     <row r="8">
       <c r="A8" s="2"/>
       <c r="F8" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9">
@@ -5930,24 +5930,24 @@
         <v>0.0</v>
       </c>
       <c r="E9" s="11">
-        <f> IF(B3&lt;0,-1,1) * max(0, FLOOR(1+log(abs(B3/B4),2)))</f>
-        <v>1</v>
+        <f> IF(B3&lt;0,-1,1) * max(0, FLOOR(1+log(abs(B3/B4),2),1))</f>
+        <v>7</v>
       </c>
       <c r="F9" s="1">
         <f>E9*ln(2)</f>
-        <v>0.6931471806</v>
+        <v>4.852030264</v>
       </c>
       <c r="G9" s="2">
         <f>2^-1*(2^E9+2^-E9)</f>
-        <v>1.25</v>
+        <v>64.00390625</v>
       </c>
       <c r="H9" s="2">
         <f>2^-1*(2^E9-2^-E9)</f>
-        <v>0.75</v>
+        <v>63.99609375</v>
       </c>
       <c r="I9">
         <f t="shared" ref="I9:I65" si="1">$B$4*H9-F9</f>
-        <v>0.05685281944</v>
+        <v>59.14406349</v>
       </c>
       <c r="J9">
         <f t="shared" ref="J9:J65" si="2">IF(I9&lt;$B$3,1,-1)</f>
@@ -5955,15 +5955,15 @@
       </c>
       <c r="K9">
         <f t="shared" ref="K9:K65" si="3">F9-$B$2</f>
-        <v>-1.306852819</v>
+        <v>-0.1479697361</v>
       </c>
       <c r="M9">
         <f>N9</f>
-        <v>1.231644509</v>
+        <v>4.262725095</v>
       </c>
       <c r="N9">
         <f>LN(abs(B3/B4)+1.8)</f>
-        <v>1.231644509</v>
+        <v>4.262725095</v>
       </c>
     </row>
     <row r="10">
@@ -5984,19 +5984,19 @@
       </c>
       <c r="F10" s="3">
         <f t="shared" ref="F10:F65" si="6">F9+J9*B10</f>
-        <v>2.079441542</v>
+        <v>6.238324625</v>
       </c>
       <c r="G10">
         <f t="shared" ref="G10:G65" si="7">G9*C10+J9*D10*H9</f>
-        <v>4.0625</v>
+        <v>256.0009766</v>
       </c>
       <c r="H10">
         <f t="shared" ref="H10:H65" si="8">J9*D10*G9+C10*H9</f>
-        <v>3.9375</v>
+        <v>255.9990234</v>
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
-        <v>1.858058458</v>
+        <v>249.7606988</v>
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
@@ -6004,15 +6004,15 @@
       </c>
       <c r="K10">
         <f t="shared" si="3"/>
-        <v>0.07944154168</v>
+        <v>1.238324625</v>
       </c>
       <c r="M10">
         <f t="shared" ref="M10:M36" si="9">$B$4*SINH($M9) - $B$3</f>
-        <v>-0.05933635139</v>
+        <v>-33.70864722</v>
       </c>
       <c r="N10">
         <f t="shared" ref="N10:N36" si="10">N9-($B$4*SINH(N9)-N9-$B$3)/($B$4*COSH(N9)-1)</f>
-        <v>2.733944346</v>
+        <v>5.363068788</v>
       </c>
     </row>
     <row r="11">
@@ -6033,35 +6033,35 @@
       </c>
       <c r="F11" s="3">
         <f t="shared" si="6"/>
-        <v>1.386294361</v>
+        <v>5.545177444</v>
       </c>
       <c r="G11">
         <f t="shared" si="7"/>
-        <v>2.125</v>
+        <v>128.0019531</v>
       </c>
       <c r="H11">
         <f t="shared" si="8"/>
-        <v>1.875</v>
+        <v>127.9980469</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>0.4887056389</v>
+        <v>122.4528694</v>
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
-        <v>-0.6137056389</v>
+        <v>0.5451774445</v>
       </c>
       <c r="M11">
         <f t="shared" si="9"/>
-        <v>-1.686231584</v>
+        <v>-217996482534310</v>
       </c>
       <c r="N11">
         <f t="shared" si="10"/>
-        <v>2.243032393</v>
+        <v>5.059158933</v>
       </c>
     </row>
     <row r="12">
@@ -6082,35 +6082,35 @@
       </c>
       <c r="F12" s="3">
         <f t="shared" si="6"/>
-        <v>1.732867951</v>
+        <v>5.198603854</v>
       </c>
       <c r="G12">
         <f t="shared" si="7"/>
-        <v>2.916815472</v>
+        <v>90.51243013</v>
       </c>
       <c r="H12">
         <f t="shared" si="8"/>
-        <v>2.740038777</v>
+        <v>90.50690586</v>
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>1.007170826</v>
+        <v>85.308302</v>
       </c>
       <c r="J12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K12">
         <f t="shared" si="3"/>
-        <v>-0.2671320486</v>
-      </c>
-      <c r="M12">
+        <v>0.1986038542</v>
+      </c>
+      <c r="M12" t="str">
         <f t="shared" si="9"/>
-        <v>-4.233800457</v>
+        <v>#NUM!</v>
       </c>
       <c r="N12">
         <f t="shared" si="10"/>
-        <v>2.033688865</v>
+        <v>5.001737818</v>
       </c>
     </row>
     <row r="13">
@@ -6131,35 +6131,35 @@
       </c>
       <c r="F13" s="3">
         <f t="shared" si="6"/>
-        <v>1.906154747</v>
+        <v>5.025317059</v>
       </c>
       <c r="G13">
         <f t="shared" si="7"/>
-        <v>3.437911106</v>
+        <v>76.11254011</v>
       </c>
       <c r="H13">
         <f t="shared" si="8"/>
-        <v>3.289260216</v>
+        <v>76.10597061</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>1.38310547</v>
+        <v>71.08065355</v>
       </c>
       <c r="J13">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K13">
         <f t="shared" si="3"/>
-        <v>-0.09384525346</v>
-      </c>
-      <c r="M13">
+        <v>0.02531705906</v>
+      </c>
+      <c r="M13" t="str">
         <f t="shared" si="9"/>
-        <v>-36.10905477</v>
+        <v>#NUM!</v>
       </c>
       <c r="N13">
         <f t="shared" si="10"/>
-        <v>2.000729826</v>
+        <v>5.00000153</v>
       </c>
     </row>
     <row r="14">
@@ -6180,19 +6180,19 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" si="6"/>
-        <v>1.992798144</v>
+        <v>4.938673661</v>
       </c>
       <c r="G14">
         <f t="shared" si="7"/>
-        <v>3.736172906</v>
+        <v>69.79607694</v>
       </c>
       <c r="H14">
         <f t="shared" si="8"/>
-        <v>3.59985944</v>
+        <v>69.78891284</v>
       </c>
       <c r="I14">
         <f t="shared" si="1"/>
-        <v>1.607061295</v>
+        <v>64.85023918</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
@@ -6200,15 +6200,15 @@
       </c>
       <c r="K14">
         <f t="shared" si="3"/>
-        <v>-0.00720185589</v>
-      </c>
-      <c r="M14">
+        <v>-0.06132633851</v>
+      </c>
+      <c r="M14" t="str">
         <f t="shared" si="9"/>
-        <v>-2.40399E+15</v>
+        <v>#NUM!</v>
       </c>
       <c r="N14">
         <f t="shared" si="10"/>
-        <v>2.00000035</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -6229,27 +6229,27 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" si="6"/>
-        <v>2.036119843</v>
+        <v>4.98199536</v>
       </c>
       <c r="G15">
         <f t="shared" si="7"/>
-        <v>3.895680234</v>
+        <v>72.8859028</v>
       </c>
       <c r="H15">
         <f t="shared" si="8"/>
-        <v>3.765146011</v>
+        <v>72.87904244</v>
       </c>
       <c r="I15">
         <f t="shared" si="1"/>
-        <v>1.729026168</v>
+        <v>67.89704708</v>
       </c>
       <c r="J15">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K15">
         <f t="shared" si="3"/>
-        <v>0.03611984289</v>
+        <v>-0.01800463973</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="9"/>
@@ -6257,7 +6257,7 @@
       </c>
       <c r="N15">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -6278,19 +6278,19 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" si="6"/>
-        <v>2.014458994</v>
+        <v>5.00365621</v>
       </c>
       <c r="G16">
         <f t="shared" si="7"/>
-        <v>3.815031543</v>
+        <v>74.48174764</v>
       </c>
       <c r="H16">
         <f t="shared" si="8"/>
-        <v>3.681638993</v>
+        <v>74.47503428</v>
       </c>
       <c r="I16">
         <f t="shared" si="1"/>
-        <v>1.66718</v>
+        <v>69.47137807</v>
       </c>
       <c r="J16">
         <f t="shared" si="2"/>
@@ -6298,7 +6298,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="3"/>
-        <v>0.0144589935</v>
+        <v>0.003656209667</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="9"/>
@@ -6306,7 +6306,7 @@
       </c>
       <c r="N16">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -6327,27 +6327,27 @@
       </c>
       <c r="F17" s="3">
         <f t="shared" si="6"/>
-        <v>2.003628569</v>
+        <v>4.992825785</v>
       </c>
       <c r="G17">
         <f t="shared" si="7"/>
-        <v>3.7753808</v>
+        <v>73.67950395</v>
       </c>
       <c r="H17">
         <f t="shared" si="8"/>
-        <v>3.6405357</v>
+        <v>73.67271749</v>
       </c>
       <c r="I17">
         <f t="shared" si="1"/>
-        <v>1.636907132</v>
+        <v>68.6798917</v>
       </c>
       <c r="J17">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K17">
         <f t="shared" si="3"/>
-        <v>0.003628568806</v>
+        <v>-0.007174215029</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="9"/>
@@ -6355,7 +6355,7 @@
       </c>
       <c r="N17">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -6376,19 +6376,19 @@
       </c>
       <c r="F18" s="3">
         <f t="shared" si="6"/>
-        <v>1.998213356</v>
+        <v>4.998240997</v>
       </c>
       <c r="G18">
         <f t="shared" si="7"/>
-        <v>3.755721786</v>
+        <v>74.07953962</v>
       </c>
       <c r="H18">
         <f t="shared" si="8"/>
-        <v>3.62014449</v>
+        <v>74.07278981</v>
       </c>
       <c r="I18">
         <f t="shared" si="1"/>
-        <v>1.621931134</v>
+        <v>69.07454881</v>
       </c>
       <c r="J18">
         <f t="shared" si="2"/>
@@ -6396,7 +6396,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="3"/>
-        <v>-0.001786643542</v>
+        <v>-0.001759002681</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="9"/>
@@ -6404,7 +6404,7 @@
       </c>
       <c r="N18">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -6425,19 +6425,19 @@
       </c>
       <c r="F19" s="3">
         <f t="shared" si="6"/>
-        <v>2.000920963</v>
+        <v>5.000948603</v>
       </c>
       <c r="G19">
         <f t="shared" si="7"/>
-        <v>3.76553749</v>
+        <v>74.28037135</v>
       </c>
       <c r="H19">
         <f t="shared" si="8"/>
-        <v>3.630326788</v>
+        <v>74.27363979</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
-        <v>1.629405825</v>
+        <v>69.27269119</v>
       </c>
       <c r="J19">
         <f t="shared" si="2"/>
@@ -6445,7 +6445,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="3"/>
-        <v>0.000920962632</v>
+        <v>0.000948603493</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="9"/>
@@ -6453,7 +6453,7 @@
       </c>
       <c r="N19">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
@@ -6474,19 +6474,19 @@
       </c>
       <c r="F20" s="3">
         <f t="shared" si="6"/>
-        <v>1.99956716</v>
+        <v>4.9995948</v>
       </c>
       <c r="G20">
         <f t="shared" si="7"/>
-        <v>3.760626192</v>
+        <v>74.17988751</v>
       </c>
       <c r="H20">
         <f t="shared" si="8"/>
-        <v>3.625232317</v>
+        <v>74.17314683</v>
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
-        <v>1.625665158</v>
+        <v>69.17355203</v>
       </c>
       <c r="J20">
         <f t="shared" si="2"/>
@@ -6494,7 +6494,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="3"/>
-        <v>-0.000432840455</v>
+        <v>-0.000405199594</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="9"/>
@@ -6502,7 +6502,7 @@
       </c>
       <c r="N20">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
@@ -6523,19 +6523,19 @@
       </c>
       <c r="F21" s="3">
         <f t="shared" si="6"/>
-        <v>2.000244061</v>
+        <v>5.000271702</v>
       </c>
       <c r="G21">
         <f t="shared" si="7"/>
-        <v>3.763080979</v>
+        <v>74.23011242</v>
       </c>
       <c r="H21">
         <f t="shared" si="8"/>
-        <v>3.627778721</v>
+        <v>74.2233763</v>
       </c>
       <c r="I21">
         <f t="shared" si="1"/>
-        <v>1.62753466</v>
+        <v>69.2231046</v>
       </c>
       <c r="J21">
         <f t="shared" si="2"/>
@@ -6543,7 +6543,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="3"/>
-        <v>0.0002440610885</v>
+        <v>0.0002717019495</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="9"/>
@@ -6551,7 +6551,7 @@
       </c>
       <c r="N21">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
@@ -6572,19 +6572,19 @@
       </c>
       <c r="F22" s="3">
         <f t="shared" si="6"/>
-        <v>1.99990561</v>
+        <v>4.999933251</v>
       </c>
       <c r="G22">
         <f t="shared" si="7"/>
-        <v>3.76185337</v>
+        <v>74.20499571</v>
       </c>
       <c r="H22">
         <f t="shared" si="8"/>
-        <v>3.626505312</v>
+        <v>74.19825732</v>
       </c>
       <c r="I22">
         <f t="shared" si="1"/>
-        <v>1.626599701</v>
+        <v>69.19832407</v>
       </c>
       <c r="J22">
         <f t="shared" si="2"/>
@@ -6592,7 +6592,7 @@
       </c>
       <c r="K22">
         <f t="shared" si="3"/>
-        <v>-0.00009438968324</v>
+        <v>-0.00006674882223</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="9"/>
@@ -6600,7 +6600,7 @@
       </c>
       <c r="N22">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
@@ -6621,19 +6621,19 @@
       </c>
       <c r="F23" s="3">
         <f t="shared" si="6"/>
-        <v>2.000074836</v>
+        <v>5.000102477</v>
       </c>
       <c r="G23">
         <f t="shared" si="7"/>
-        <v>3.76246712</v>
+        <v>74.217553</v>
       </c>
       <c r="H23">
         <f t="shared" si="8"/>
-        <v>3.627141965</v>
+        <v>74.21081575</v>
       </c>
       <c r="I23">
         <f t="shared" si="1"/>
-        <v>1.627067129</v>
+        <v>69.21071327</v>
       </c>
       <c r="J23">
         <f t="shared" si="2"/>
@@ -6641,7 +6641,7 @@
       </c>
       <c r="K23">
         <f t="shared" si="3"/>
-        <v>0.00007483570263</v>
+        <v>0.0001024765636</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="9"/>
@@ -6649,7 +6649,7 @@
       </c>
       <c r="N23">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
@@ -6670,27 +6670,27 @@
       </c>
       <c r="F24" s="3">
         <f t="shared" si="6"/>
-        <v>1.999990223</v>
+        <v>5.000017864</v>
       </c>
       <c r="G24">
         <f t="shared" si="7"/>
-        <v>3.762160231</v>
+        <v>74.21127409</v>
       </c>
       <c r="H24">
         <f t="shared" si="8"/>
-        <v>3.626823625</v>
+        <v>74.20453627</v>
       </c>
       <c r="I24">
         <f t="shared" si="1"/>
-        <v>1.626833402</v>
+        <v>69.2045184</v>
       </c>
       <c r="J24">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K24">
         <f t="shared" si="3"/>
-        <v>-0.000009776990305</v>
+        <v>0.00001786387071</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="9"/>
@@ -6698,7 +6698,7 @@
       </c>
       <c r="N24">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
@@ -6719,27 +6719,27 @@
       </c>
       <c r="F25" s="3">
         <f t="shared" si="6"/>
-        <v>2.000032529</v>
+        <v>4.999975558</v>
       </c>
       <c r="G25">
         <f t="shared" si="7"/>
-        <v>3.762313673</v>
+        <v>74.20813484</v>
       </c>
       <c r="H25">
         <f t="shared" si="8"/>
-        <v>3.626982792</v>
+        <v>74.20139673</v>
       </c>
       <c r="I25">
         <f t="shared" si="1"/>
-        <v>1.626950262</v>
+        <v>69.20142117</v>
       </c>
       <c r="J25">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K25">
         <f t="shared" si="3"/>
-        <v>0.00003252935617</v>
+        <v>-0.00002444247576</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="9"/>
@@ -6747,7 +6747,7 @@
       </c>
       <c r="N25">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
@@ -6768,27 +6768,27 @@
       </c>
       <c r="F26" s="3">
         <f t="shared" si="6"/>
-        <v>2.000011376</v>
+        <v>4.999996711</v>
       </c>
       <c r="G26">
         <f t="shared" si="7"/>
-        <v>3.762236951</v>
+        <v>74.20970445</v>
       </c>
       <c r="H26">
         <f t="shared" si="8"/>
-        <v>3.626903208</v>
+        <v>74.20296648</v>
       </c>
       <c r="I26">
         <f t="shared" si="1"/>
-        <v>1.626891831</v>
+        <v>69.20296977</v>
       </c>
       <c r="J26">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K26">
         <f t="shared" si="3"/>
-        <v>0.00001137618293</v>
+        <v>-0.000003289302526</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="9"/>
@@ -6796,7 +6796,7 @@
       </c>
       <c r="N26">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -6817,19 +6817,19 @@
       </c>
       <c r="F27" s="3">
         <f t="shared" si="6"/>
-        <v>2.0000008</v>
+        <v>5.000007287</v>
       </c>
       <c r="G27">
         <f t="shared" si="7"/>
-        <v>3.762198591</v>
+        <v>74.21048927</v>
       </c>
       <c r="H27">
         <f t="shared" si="8"/>
-        <v>3.626863416</v>
+        <v>74.20375137</v>
       </c>
       <c r="I27">
         <f t="shared" si="1"/>
-        <v>1.626862616</v>
+        <v>69.20374408</v>
       </c>
       <c r="J27">
         <f t="shared" si="2"/>
@@ -6837,7 +6837,7 @@
       </c>
       <c r="K27">
         <f t="shared" si="3"/>
-        <v>0.0000007995963127</v>
+        <v>0.000007287284091</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="9"/>
@@ -6845,7 +6845,7 @@
       </c>
       <c r="N27">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
@@ -6866,27 +6866,27 @@
       </c>
       <c r="F28" s="3">
         <f t="shared" si="6"/>
-        <v>1.999995511</v>
+        <v>5.000001999</v>
       </c>
       <c r="G28">
         <f t="shared" si="7"/>
-        <v>3.762179411</v>
+        <v>74.21009686</v>
       </c>
       <c r="H28">
         <f t="shared" si="8"/>
-        <v>3.626843521</v>
+        <v>74.20335892</v>
       </c>
       <c r="I28">
         <f t="shared" si="1"/>
-        <v>1.626848009</v>
+        <v>69.20335692</v>
       </c>
       <c r="J28">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K28">
         <f t="shared" si="3"/>
-        <v>-0.000004488696996</v>
+        <v>0.000001998990782</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="9"/>
@@ -6894,7 +6894,7 @@
       </c>
       <c r="N28">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
@@ -6915,19 +6915,19 @@
       </c>
       <c r="F29" s="3">
         <f t="shared" si="6"/>
-        <v>1.999998155</v>
+        <v>4.999999355</v>
       </c>
       <c r="G29">
         <f t="shared" si="7"/>
-        <v>3.762189001</v>
+        <v>74.20990065</v>
       </c>
       <c r="H29">
         <f t="shared" si="8"/>
-        <v>3.626853468</v>
+        <v>74.2031627</v>
       </c>
       <c r="I29">
         <f t="shared" si="1"/>
-        <v>1.626855313</v>
+        <v>69.20316335</v>
       </c>
       <c r="J29">
         <f t="shared" si="2"/>
@@ -6935,7 +6935,7 @@
       </c>
       <c r="K29">
         <f t="shared" si="3"/>
-        <v>-0.000001844550342</v>
+        <v>-0.0000006451558727</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="9"/>
@@ -6943,7 +6943,7 @@
       </c>
       <c r="N29">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
@@ -6964,27 +6964,27 @@
       </c>
       <c r="F30" s="3">
         <f t="shared" si="6"/>
-        <v>1.999999478</v>
+        <v>5.000000677</v>
       </c>
       <c r="G30">
         <f t="shared" si="7"/>
-        <v>3.762193796</v>
+        <v>74.20999875</v>
       </c>
       <c r="H30">
         <f t="shared" si="8"/>
-        <v>3.626858442</v>
+        <v>74.20326081</v>
       </c>
       <c r="I30">
         <f t="shared" si="1"/>
-        <v>1.626858965</v>
+        <v>69.20326013</v>
       </c>
       <c r="J30">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K30">
         <f t="shared" si="3"/>
-        <v>-0.0000005224770145</v>
+        <v>0.0000006769174545</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="9"/>
@@ -6992,7 +6992,7 @@
       </c>
       <c r="N30">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
@@ -7013,19 +7013,19 @@
       </c>
       <c r="F31" s="3">
         <f t="shared" si="6"/>
-        <v>2.000000139</v>
+        <v>5.000000016</v>
       </c>
       <c r="G31">
         <f t="shared" si="7"/>
-        <v>3.762196194</v>
+        <v>74.2099497</v>
       </c>
       <c r="H31">
         <f t="shared" si="8"/>
-        <v>3.626860929</v>
+        <v>74.20321176</v>
       </c>
       <c r="I31">
         <f t="shared" si="1"/>
-        <v>1.626860791</v>
+        <v>69.20321174</v>
       </c>
       <c r="J31">
         <f t="shared" si="2"/>
@@ -7033,7 +7033,7 @@
       </c>
       <c r="K31">
         <f t="shared" si="3"/>
-        <v>0.0000001385596491</v>
+        <v>0.0000000158807909</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" si="9"/>
@@ -7041,7 +7041,7 @@
       </c>
       <c r="N31">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32">
@@ -7062,19 +7062,19 @@
       </c>
       <c r="F32" s="3">
         <f t="shared" si="6"/>
-        <v>1.999999808</v>
+        <v>4.999999685</v>
       </c>
       <c r="G32">
         <f t="shared" si="7"/>
-        <v>3.762194995</v>
+        <v>74.20992518</v>
       </c>
       <c r="H32">
         <f t="shared" si="8"/>
-        <v>3.626859686</v>
+        <v>74.20318723</v>
       </c>
       <c r="I32">
         <f t="shared" si="1"/>
-        <v>1.626859878</v>
+        <v>69.20318754</v>
       </c>
       <c r="J32">
         <f t="shared" si="2"/>
@@ -7082,7 +7082,7 @@
       </c>
       <c r="K32">
         <f t="shared" si="3"/>
-        <v>-0.0000001919586827</v>
+        <v>-0.0000003146375409</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" si="9"/>
@@ -7090,7 +7090,7 @@
       </c>
       <c r="N32">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
@@ -7111,19 +7111,19 @@
       </c>
       <c r="F33" s="3">
         <f t="shared" si="6"/>
-        <v>1.999999973</v>
+        <v>4.999999851</v>
       </c>
       <c r="G33">
         <f t="shared" si="7"/>
-        <v>3.762195594</v>
+        <v>74.20993744</v>
       </c>
       <c r="H33">
         <f t="shared" si="8"/>
-        <v>3.626860307</v>
+        <v>74.20319949</v>
       </c>
       <c r="I33">
         <f t="shared" si="1"/>
-        <v>1.626860334</v>
+        <v>69.20319964</v>
       </c>
       <c r="J33">
         <f t="shared" si="2"/>
@@ -7131,7 +7131,7 @@
       </c>
       <c r="K33">
         <f t="shared" si="3"/>
-        <v>-0.00000002669951682</v>
+        <v>-0.0000001493783754</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" si="9"/>
@@ -7139,7 +7139,7 @@
       </c>
       <c r="N33">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
@@ -7160,27 +7160,27 @@
       </c>
       <c r="F34" s="3">
         <f t="shared" si="6"/>
-        <v>2.000000056</v>
+        <v>4.999999933</v>
       </c>
       <c r="G34">
         <f t="shared" si="7"/>
-        <v>3.762195894</v>
+        <v>74.20994357</v>
       </c>
       <c r="H34">
         <f t="shared" si="8"/>
-        <v>3.626860618</v>
+        <v>74.20320562</v>
       </c>
       <c r="I34">
         <f t="shared" si="1"/>
-        <v>1.626860562</v>
+        <v>69.20320569</v>
       </c>
       <c r="J34">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K34">
         <f t="shared" si="3"/>
-        <v>0.00000005593006591</v>
+        <v>-0.00000006674879227</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" si="9"/>
@@ -7188,7 +7188,7 @@
       </c>
       <c r="N34">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35">
@@ -7209,27 +7209,27 @@
       </c>
       <c r="F35" s="3">
         <f t="shared" si="6"/>
-        <v>2.000000015</v>
+        <v>4.999999975</v>
       </c>
       <c r="G35">
         <f t="shared" si="7"/>
-        <v>3.762195744</v>
+        <v>74.20994664</v>
       </c>
       <c r="H35">
         <f t="shared" si="8"/>
-        <v>3.626860463</v>
+        <v>74.20320869</v>
       </c>
       <c r="I35">
         <f t="shared" si="1"/>
-        <v>1.626860448</v>
+        <v>69.20320872</v>
       </c>
       <c r="J35">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K35">
         <f t="shared" si="3"/>
-        <v>0.00000001461527432</v>
+        <v>-0.00000002543400068</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" si="9"/>
@@ -7237,7 +7237,7 @@
       </c>
       <c r="N35">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36">
@@ -7258,19 +7258,19 @@
       </c>
       <c r="F36" s="3">
         <f t="shared" si="6"/>
-        <v>1.999999994</v>
+        <v>4.999999995</v>
       </c>
       <c r="G36">
         <f t="shared" si="7"/>
-        <v>3.762195669</v>
+        <v>74.20994817</v>
       </c>
       <c r="H36">
         <f t="shared" si="8"/>
-        <v>3.626860385</v>
+        <v>74.20321022</v>
       </c>
       <c r="I36">
         <f t="shared" si="1"/>
-        <v>1.626860391</v>
+        <v>69.20321023</v>
       </c>
       <c r="J36">
         <f t="shared" si="2"/>
@@ -7278,7 +7278,7 @@
       </c>
       <c r="K36">
         <f t="shared" si="3"/>
-        <v>-0.00000000604212147</v>
+        <v>-0.000000004776604889</v>
       </c>
       <c r="M36" t="str">
         <f t="shared" si="9"/>
@@ -7286,7 +7286,7 @@
       </c>
       <c r="N36">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
@@ -7307,19 +7307,19 @@
       </c>
       <c r="F37" s="3">
         <f t="shared" si="6"/>
-        <v>2.000000004</v>
+        <v>5.000000006</v>
       </c>
       <c r="G37">
         <f t="shared" si="7"/>
-        <v>3.762195707</v>
+        <v>74.20994894</v>
       </c>
       <c r="H37">
         <f t="shared" si="8"/>
-        <v>3.626860424</v>
+        <v>74.20321099</v>
       </c>
       <c r="I37">
         <f t="shared" si="1"/>
-        <v>1.62686042</v>
+        <v>69.20321098</v>
       </c>
       <c r="J37">
         <f t="shared" si="2"/>
@@ -7327,7 +7327,7 @@
       </c>
       <c r="K37">
         <f t="shared" si="3"/>
-        <v>0.000000004286576427</v>
+        <v>0.000000005552093008</v>
       </c>
     </row>
     <row r="38">
@@ -7348,27 +7348,27 @@
       </c>
       <c r="F38" s="3">
         <f t="shared" si="6"/>
-        <v>1.999999999</v>
+        <v>5</v>
       </c>
       <c r="G38">
         <f t="shared" si="7"/>
-        <v>3.762195688</v>
+        <v>74.20994855</v>
       </c>
       <c r="H38">
         <f t="shared" si="8"/>
-        <v>3.626860405</v>
+        <v>74.20321061</v>
       </c>
       <c r="I38">
         <f t="shared" si="1"/>
-        <v>1.626860405</v>
+        <v>69.20321061</v>
       </c>
       <c r="J38">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K38">
         <f t="shared" si="3"/>
-        <v>-0.0000000008777725213</v>
+        <v>0.0000000003877440591</v>
       </c>
     </row>
     <row r="39">
@@ -7389,27 +7389,27 @@
       </c>
       <c r="F39" s="3">
         <f t="shared" si="6"/>
-        <v>2.000000002</v>
+        <v>4.999999998</v>
       </c>
       <c r="G39">
         <f t="shared" si="7"/>
-        <v>3.762195697</v>
+        <v>74.20994836</v>
       </c>
       <c r="H39">
         <f t="shared" si="8"/>
-        <v>3.626860414</v>
+        <v>74.20321041</v>
       </c>
       <c r="I39">
         <f t="shared" si="1"/>
-        <v>1.626860413</v>
+        <v>69.20321042</v>
       </c>
       <c r="J39">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K39">
         <f t="shared" si="3"/>
-        <v>0.000000001704401953</v>
+        <v>-0.000000002194430415</v>
       </c>
     </row>
     <row r="40">
@@ -7430,27 +7430,27 @@
       </c>
       <c r="F40" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>4.999999999</v>
       </c>
       <c r="G40">
         <f t="shared" si="7"/>
-        <v>3.762195693</v>
+        <v>74.20994846</v>
       </c>
       <c r="H40">
         <f t="shared" si="8"/>
-        <v>3.626860409</v>
+        <v>74.20321051</v>
       </c>
       <c r="I40">
         <f t="shared" si="1"/>
-        <v>1.626860409</v>
+        <v>69.20321051</v>
       </c>
       <c r="J40">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K40">
         <f t="shared" si="3"/>
-        <v>0.0000000004133147158</v>
+        <v>-0.000000000903343178</v>
       </c>
     </row>
     <row r="41">
@@ -7471,19 +7471,19 @@
       </c>
       <c r="F41" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G41">
         <f t="shared" si="7"/>
-        <v>3.76219569</v>
+        <v>74.20994851</v>
       </c>
       <c r="H41">
         <f t="shared" si="8"/>
-        <v>3.626860407</v>
+        <v>74.20321056</v>
       </c>
       <c r="I41">
         <f t="shared" si="1"/>
-        <v>1.626860407</v>
+        <v>69.20321056</v>
       </c>
       <c r="J41">
         <f t="shared" si="2"/>
@@ -7491,7 +7491,7 @@
       </c>
       <c r="K41">
         <f t="shared" si="3"/>
-        <v>-0.0000000002322289028</v>
+        <v>-0.0000000002578000036</v>
       </c>
     </row>
     <row r="42">
@@ -7512,19 +7512,19 @@
       </c>
       <c r="F42" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G42">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994853</v>
       </c>
       <c r="H42">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I42">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J42">
         <f t="shared" si="2"/>
@@ -7553,19 +7553,19 @@
       </c>
       <c r="F43" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G43">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H43">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321057</v>
       </c>
       <c r="I43">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321057</v>
       </c>
       <c r="J43">
         <f t="shared" si="2"/>
@@ -7594,23 +7594,23 @@
       </c>
       <c r="F44" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G44">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H44">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I44">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J44">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K44">
         <f t="shared" si="3"/>
@@ -7635,23 +7635,23 @@
       </c>
       <c r="F45" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G45">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994853</v>
       </c>
       <c r="H45">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I45">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J45">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K45">
         <f t="shared" si="3"/>
@@ -7676,23 +7676,23 @@
       </c>
       <c r="F46" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G46">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994853</v>
       </c>
       <c r="H46">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I46">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J46">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K46">
         <f t="shared" si="3"/>
@@ -7717,19 +7717,19 @@
       </c>
       <c r="F47" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G47">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H47">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I47">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J47">
         <f t="shared" si="2"/>
@@ -7758,23 +7758,23 @@
       </c>
       <c r="F48" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G48">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H48">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I48">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J48">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K48">
         <f t="shared" si="3"/>
@@ -7799,19 +7799,19 @@
       </c>
       <c r="F49" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G49">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H49">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I49">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J49">
         <f t="shared" si="2"/>
@@ -7840,19 +7840,19 @@
       </c>
       <c r="F50" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G50">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H50">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I50">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J50">
         <f t="shared" si="2"/>
@@ -7881,19 +7881,19 @@
       </c>
       <c r="F51" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G51">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H51">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I51">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J51">
         <f t="shared" si="2"/>
@@ -7922,23 +7922,23 @@
       </c>
       <c r="F52" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G52">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H52">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I52">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J52">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K52">
         <f t="shared" si="3"/>
@@ -7963,19 +7963,19 @@
       </c>
       <c r="F53" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G53">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H53">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I53">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J53">
         <f t="shared" si="2"/>
@@ -8004,23 +8004,23 @@
       </c>
       <c r="F54" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G54">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H54">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I54">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J54">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K54">
         <f t="shared" si="3"/>
@@ -8045,23 +8045,23 @@
       </c>
       <c r="F55" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G55">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H55">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I55">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J55">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K55">
         <f t="shared" si="3"/>
@@ -8086,19 +8086,19 @@
       </c>
       <c r="F56" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G56">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H56">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I56">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J56">
         <f t="shared" si="2"/>
@@ -8127,19 +8127,19 @@
       </c>
       <c r="F57" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G57">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H57">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I57">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J57">
         <f t="shared" si="2"/>
@@ -8168,19 +8168,19 @@
       </c>
       <c r="F58" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G58">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H58">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I58">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J58">
         <f t="shared" si="2"/>
@@ -8209,19 +8209,19 @@
       </c>
       <c r="F59" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G59">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H59">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I59">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J59">
         <f t="shared" si="2"/>
@@ -8250,23 +8250,23 @@
       </c>
       <c r="F60" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G60">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H60">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I60">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J60">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K60">
         <f t="shared" si="3"/>
@@ -8291,23 +8291,23 @@
       </c>
       <c r="F61" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G61">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H61">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I61">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J61">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K61">
         <f t="shared" si="3"/>
@@ -8332,19 +8332,19 @@
       </c>
       <c r="F62" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G62">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H62">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I62">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J62">
         <f t="shared" si="2"/>
@@ -8373,23 +8373,23 @@
       </c>
       <c r="F63" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G63">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H63">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I63">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J63">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K63">
         <f t="shared" si="3"/>
@@ -8414,19 +8414,19 @@
       </c>
       <c r="F64" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G64">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H64">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I64">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J64">
         <f t="shared" si="2"/>
@@ -8455,19 +8455,19 @@
       </c>
       <c r="F65" s="3">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G65">
         <f t="shared" si="7"/>
-        <v>3.762195691</v>
+        <v>74.20994852</v>
       </c>
       <c r="H65">
         <f t="shared" si="8"/>
-        <v>3.626860408</v>
+        <v>74.20321058</v>
       </c>
       <c r="I65">
         <f t="shared" si="1"/>
-        <v>1.626860408</v>
+        <v>69.20321058</v>
       </c>
       <c r="J65">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Hyperbolic E renamed to H. Set back: H=2.
</commit_message>
<xml_diff>
--- a/xlsx/ke.xlsx
+++ b/xlsx/ke.xlsx
@@ -12,9 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Solving Kepler's equation M = E - e sinE</t>
+  </si>
+  <si>
+    <t>Solving Kepler's equation (hyperbolic case) M = e sinh H - H</t>
   </si>
   <si>
     <t>E:</t>
@@ -92,16 +95,16 @@
     <t>E_0 = M + 0.85e</t>
   </si>
   <si>
-    <t>Solving Kepler's equation (hyperbolic case) M = e sinh E - E</t>
+    <t>H:</t>
   </si>
   <si>
-    <t>cosh E:</t>
+    <t>cosh H:</t>
   </si>
   <si>
-    <t>sinh E:</t>
+    <t>sinh H:</t>
   </si>
   <si>
-    <t>e*exp(E)/2:</t>
+    <t>e*exp(H)/2:</t>
   </si>
   <si>
     <t>cosh a_n</t>
@@ -113,19 +116,31 @@
     <t>m</t>
   </si>
   <si>
-    <t>cosh E_n</t>
+    <t>Hn</t>
   </si>
   <si>
-    <t>sinh E_n</t>
+    <t>cosh H_n</t>
   </si>
   <si>
-    <t>e*sinh E_n - E_n</t>
+    <t>sinh H_n</t>
   </si>
   <si>
-    <t>E_n+1 = e*sinh E_n - M</t>
+    <t>H_n - H</t>
   </si>
   <si>
-    <t>E_0 = log(abs(M/e) + 1.8)</t>
+    <t>H_n</t>
+  </si>
+  <si>
+    <t>H_n-1 + s_n*a_n</t>
+  </si>
+  <si>
+    <t>e*sinh H_n - H_n</t>
+  </si>
+  <si>
+    <t>H_n+1 = e*sinh H_n - M</t>
+  </si>
+  <si>
+    <t>H_0 = log(abs(M/e) + 1.8)</t>
   </si>
 </sst>
 </file>
@@ -256,20 +271,20 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="5">
         <v>2.0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2">
         <f>cos(B2)</f>
         <v>-0.4161468365</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2">
         <f>sin(B2)</f>
@@ -278,7 +293,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="6">
         <f>B2-B4*sin(B2)</f>
@@ -288,7 +303,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="5">
         <v>1.0</v>
@@ -297,13 +312,13 @@
     </row>
     <row r="5">
       <c r="F5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -335,42 +350,42 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
@@ -388,23 +403,23 @@
     <row r="8">
       <c r="A8" s="2"/>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
@@ -5756,7 +5771,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -5764,40 +5779,40 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B2" s="5">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2">
         <f> COSH(B2)</f>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2">
         <f> SINH(B2)</f>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="6">
         <f> B4*SINH(B2) - B2</f>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <f> exp(B2)/2*B4</f>
-        <v>74.20657955</v>
+        <v>3.694528049</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="10"/>
@@ -5805,7 +5820,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="5">
         <v>1.0</v>
@@ -5815,13 +5830,13 @@
     </row>
     <row r="5">
       <c r="F5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -5853,44 +5868,44 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="7" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
@@ -5908,21 +5923,21 @@
     <row r="8">
       <c r="A8" s="2"/>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
@@ -5931,23 +5946,23 @@
       </c>
       <c r="E9" s="11">
         <f> IF(B3&lt;0,-1,1) * max(0, FLOOR(1+log(abs(B3/B4),2),1))</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1">
         <f>E9*ln(2)</f>
-        <v>4.852030264</v>
+        <v>0.6931471806</v>
       </c>
       <c r="G9" s="2">
         <f>2^-1*(2^E9+2^-E9)</f>
-        <v>64.00390625</v>
+        <v>1.25</v>
       </c>
       <c r="H9" s="2">
         <f>2^-1*(2^E9-2^-E9)</f>
-        <v>63.99609375</v>
+        <v>0.75</v>
       </c>
       <c r="I9">
         <f t="shared" ref="I9:I65" si="1">$B$4*H9-F9</f>
-        <v>59.14406349</v>
+        <v>0.05685281944</v>
       </c>
       <c r="J9">
         <f t="shared" ref="J9:J65" si="2">IF(I9&lt;$B$3,1,-1)</f>
@@ -5955,15 +5970,15 @@
       </c>
       <c r="K9">
         <f t="shared" ref="K9:K65" si="3">F9-$B$2</f>
-        <v>-0.1479697361</v>
+        <v>-1.306852819</v>
       </c>
       <c r="M9">
         <f>N9</f>
-        <v>4.262725095</v>
+        <v>1.231644509</v>
       </c>
       <c r="N9">
         <f>LN(abs(B3/B4)+1.8)</f>
-        <v>4.262725095</v>
+        <v>1.231644509</v>
       </c>
     </row>
     <row r="10">
@@ -5984,19 +5999,19 @@
       </c>
       <c r="F10" s="3">
         <f t="shared" ref="F10:F65" si="6">F9+J9*B10</f>
-        <v>6.238324625</v>
+        <v>2.079441542</v>
       </c>
       <c r="G10">
         <f t="shared" ref="G10:G65" si="7">G9*C10+J9*D10*H9</f>
-        <v>256.0009766</v>
+        <v>4.0625</v>
       </c>
       <c r="H10">
         <f t="shared" ref="H10:H65" si="8">J9*D10*G9+C10*H9</f>
-        <v>255.9990234</v>
+        <v>3.9375</v>
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
-        <v>249.7606988</v>
+        <v>1.858058458</v>
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
@@ -6004,15 +6019,15 @@
       </c>
       <c r="K10">
         <f t="shared" si="3"/>
-        <v>1.238324625</v>
+        <v>0.07944154168</v>
       </c>
       <c r="M10">
         <f t="shared" ref="M10:M36" si="9">$B$4*SINH($M9) - $B$3</f>
-        <v>-33.70864722</v>
+        <v>-0.05933635139</v>
       </c>
       <c r="N10">
         <f t="shared" ref="N10:N36" si="10">N9-($B$4*SINH(N9)-N9-$B$3)/($B$4*COSH(N9)-1)</f>
-        <v>5.363068788</v>
+        <v>2.733944346</v>
       </c>
     </row>
     <row r="11">
@@ -6033,35 +6048,35 @@
       </c>
       <c r="F11" s="3">
         <f t="shared" si="6"/>
-        <v>5.545177444</v>
+        <v>1.386294361</v>
       </c>
       <c r="G11">
         <f t="shared" si="7"/>
-        <v>128.0019531</v>
+        <v>2.125</v>
       </c>
       <c r="H11">
         <f t="shared" si="8"/>
-        <v>127.9980469</v>
+        <v>1.875</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>122.4528694</v>
+        <v>0.4887056389</v>
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
-        <v>0.5451774445</v>
+        <v>-0.6137056389</v>
       </c>
       <c r="M11">
         <f t="shared" si="9"/>
-        <v>-217996482534310</v>
+        <v>-1.686231584</v>
       </c>
       <c r="N11">
         <f t="shared" si="10"/>
-        <v>5.059158933</v>
+        <v>2.243032393</v>
       </c>
     </row>
     <row r="12">
@@ -6082,35 +6097,35 @@
       </c>
       <c r="F12" s="3">
         <f t="shared" si="6"/>
-        <v>5.198603854</v>
+        <v>1.732867951</v>
       </c>
       <c r="G12">
         <f t="shared" si="7"/>
-        <v>90.51243013</v>
+        <v>2.916815472</v>
       </c>
       <c r="H12">
         <f t="shared" si="8"/>
-        <v>90.50690586</v>
+        <v>2.740038777</v>
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>85.308302</v>
+        <v>1.007170826</v>
       </c>
       <c r="J12">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K12">
         <f t="shared" si="3"/>
-        <v>0.1986038542</v>
-      </c>
-      <c r="M12" t="str">
+        <v>-0.2671320486</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="9"/>
-        <v>#NUM!</v>
+        <v>-4.233800457</v>
       </c>
       <c r="N12">
         <f t="shared" si="10"/>
-        <v>5.001737818</v>
+        <v>2.033688865</v>
       </c>
     </row>
     <row r="13">
@@ -6131,35 +6146,35 @@
       </c>
       <c r="F13" s="3">
         <f t="shared" si="6"/>
-        <v>5.025317059</v>
+        <v>1.906154747</v>
       </c>
       <c r="G13">
         <f t="shared" si="7"/>
-        <v>76.11254011</v>
+        <v>3.437911106</v>
       </c>
       <c r="H13">
         <f t="shared" si="8"/>
-        <v>76.10597061</v>
+        <v>3.289260216</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>71.08065355</v>
+        <v>1.38310547</v>
       </c>
       <c r="J13">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <f t="shared" si="3"/>
-        <v>0.02531705906</v>
-      </c>
-      <c r="M13" t="str">
+        <v>-0.09384525346</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="9"/>
-        <v>#NUM!</v>
+        <v>-36.10905477</v>
       </c>
       <c r="N13">
         <f t="shared" si="10"/>
-        <v>5.00000153</v>
+        <v>2.000729826</v>
       </c>
     </row>
     <row r="14">
@@ -6180,19 +6195,19 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" si="6"/>
-        <v>4.938673661</v>
+        <v>1.992798144</v>
       </c>
       <c r="G14">
         <f t="shared" si="7"/>
-        <v>69.79607694</v>
+        <v>3.736172906</v>
       </c>
       <c r="H14">
         <f t="shared" si="8"/>
-        <v>69.78891284</v>
+        <v>3.59985944</v>
       </c>
       <c r="I14">
         <f t="shared" si="1"/>
-        <v>64.85023918</v>
+        <v>1.607061295</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
@@ -6200,15 +6215,15 @@
       </c>
       <c r="K14">
         <f t="shared" si="3"/>
-        <v>-0.06132633851</v>
-      </c>
-      <c r="M14" t="str">
+        <v>-0.00720185589</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="9"/>
-        <v>#NUM!</v>
+        <v>-2.40399E+15</v>
       </c>
       <c r="N14">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2.00000035</v>
       </c>
     </row>
     <row r="15">
@@ -6229,27 +6244,27 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" si="6"/>
-        <v>4.98199536</v>
+        <v>2.036119843</v>
       </c>
       <c r="G15">
         <f t="shared" si="7"/>
-        <v>72.8859028</v>
+        <v>3.895680234</v>
       </c>
       <c r="H15">
         <f t="shared" si="8"/>
-        <v>72.87904244</v>
+        <v>3.765146011</v>
       </c>
       <c r="I15">
         <f t="shared" si="1"/>
-        <v>67.89704708</v>
+        <v>1.729026168</v>
       </c>
       <c r="J15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K15">
         <f t="shared" si="3"/>
-        <v>-0.01800463973</v>
+        <v>0.03611984289</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="9"/>
@@ -6257,7 +6272,7 @@
       </c>
       <c r="N15">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -6278,19 +6293,19 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" si="6"/>
-        <v>5.00365621</v>
+        <v>2.014458994</v>
       </c>
       <c r="G16">
         <f t="shared" si="7"/>
-        <v>74.48174764</v>
+        <v>3.815031543</v>
       </c>
       <c r="H16">
         <f t="shared" si="8"/>
-        <v>74.47503428</v>
+        <v>3.681638993</v>
       </c>
       <c r="I16">
         <f t="shared" si="1"/>
-        <v>69.47137807</v>
+        <v>1.66718</v>
       </c>
       <c r="J16">
         <f t="shared" si="2"/>
@@ -6298,7 +6313,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="3"/>
-        <v>0.003656209667</v>
+        <v>0.0144589935</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="9"/>
@@ -6306,7 +6321,7 @@
       </c>
       <c r="N16">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -6327,27 +6342,27 @@
       </c>
       <c r="F17" s="3">
         <f t="shared" si="6"/>
-        <v>4.992825785</v>
+        <v>2.003628569</v>
       </c>
       <c r="G17">
         <f t="shared" si="7"/>
-        <v>73.67950395</v>
+        <v>3.7753808</v>
       </c>
       <c r="H17">
         <f t="shared" si="8"/>
-        <v>73.67271749</v>
+        <v>3.6405357</v>
       </c>
       <c r="I17">
         <f t="shared" si="1"/>
-        <v>68.6798917</v>
+        <v>1.636907132</v>
       </c>
       <c r="J17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K17">
         <f t="shared" si="3"/>
-        <v>-0.007174215029</v>
+        <v>0.003628568806</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="9"/>
@@ -6355,7 +6370,7 @@
       </c>
       <c r="N17">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -6376,19 +6391,19 @@
       </c>
       <c r="F18" s="3">
         <f t="shared" si="6"/>
-        <v>4.998240997</v>
+        <v>1.998213356</v>
       </c>
       <c r="G18">
         <f t="shared" si="7"/>
-        <v>74.07953962</v>
+        <v>3.755721786</v>
       </c>
       <c r="H18">
         <f t="shared" si="8"/>
-        <v>74.07278981</v>
+        <v>3.62014449</v>
       </c>
       <c r="I18">
         <f t="shared" si="1"/>
-        <v>69.07454881</v>
+        <v>1.621931134</v>
       </c>
       <c r="J18">
         <f t="shared" si="2"/>
@@ -6396,7 +6411,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="3"/>
-        <v>-0.001759002681</v>
+        <v>-0.001786643542</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="9"/>
@@ -6404,7 +6419,7 @@
       </c>
       <c r="N18">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -6425,19 +6440,19 @@
       </c>
       <c r="F19" s="3">
         <f t="shared" si="6"/>
-        <v>5.000948603</v>
+        <v>2.000920963</v>
       </c>
       <c r="G19">
         <f t="shared" si="7"/>
-        <v>74.28037135</v>
+        <v>3.76553749</v>
       </c>
       <c r="H19">
         <f t="shared" si="8"/>
-        <v>74.27363979</v>
+        <v>3.630326788</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
-        <v>69.27269119</v>
+        <v>1.629405825</v>
       </c>
       <c r="J19">
         <f t="shared" si="2"/>
@@ -6445,7 +6460,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="3"/>
-        <v>0.000948603493</v>
+        <v>0.000920962632</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="9"/>
@@ -6453,7 +6468,7 @@
       </c>
       <c r="N19">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -6474,19 +6489,19 @@
       </c>
       <c r="F20" s="3">
         <f t="shared" si="6"/>
-        <v>4.9995948</v>
+        <v>1.99956716</v>
       </c>
       <c r="G20">
         <f t="shared" si="7"/>
-        <v>74.17988751</v>
+        <v>3.760626192</v>
       </c>
       <c r="H20">
         <f t="shared" si="8"/>
-        <v>74.17314683</v>
+        <v>3.625232317</v>
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
-        <v>69.17355203</v>
+        <v>1.625665158</v>
       </c>
       <c r="J20">
         <f t="shared" si="2"/>
@@ -6494,7 +6509,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="3"/>
-        <v>-0.000405199594</v>
+        <v>-0.000432840455</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="9"/>
@@ -6502,7 +6517,7 @@
       </c>
       <c r="N20">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -6523,19 +6538,19 @@
       </c>
       <c r="F21" s="3">
         <f t="shared" si="6"/>
-        <v>5.000271702</v>
+        <v>2.000244061</v>
       </c>
       <c r="G21">
         <f t="shared" si="7"/>
-        <v>74.23011242</v>
+        <v>3.763080979</v>
       </c>
       <c r="H21">
         <f t="shared" si="8"/>
-        <v>74.2233763</v>
+        <v>3.627778721</v>
       </c>
       <c r="I21">
         <f t="shared" si="1"/>
-        <v>69.2231046</v>
+        <v>1.62753466</v>
       </c>
       <c r="J21">
         <f t="shared" si="2"/>
@@ -6543,7 +6558,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="3"/>
-        <v>0.0002717019495</v>
+        <v>0.0002440610885</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="9"/>
@@ -6551,7 +6566,7 @@
       </c>
       <c r="N21">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -6572,19 +6587,19 @@
       </c>
       <c r="F22" s="3">
         <f t="shared" si="6"/>
-        <v>4.999933251</v>
+        <v>1.99990561</v>
       </c>
       <c r="G22">
         <f t="shared" si="7"/>
-        <v>74.20499571</v>
+        <v>3.76185337</v>
       </c>
       <c r="H22">
         <f t="shared" si="8"/>
-        <v>74.19825732</v>
+        <v>3.626505312</v>
       </c>
       <c r="I22">
         <f t="shared" si="1"/>
-        <v>69.19832407</v>
+        <v>1.626599701</v>
       </c>
       <c r="J22">
         <f t="shared" si="2"/>
@@ -6592,7 +6607,7 @@
       </c>
       <c r="K22">
         <f t="shared" si="3"/>
-        <v>-0.00006674882223</v>
+        <v>-0.00009438968324</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="9"/>
@@ -6600,7 +6615,7 @@
       </c>
       <c r="N22">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -6621,19 +6636,19 @@
       </c>
       <c r="F23" s="3">
         <f t="shared" si="6"/>
-        <v>5.000102477</v>
+        <v>2.000074836</v>
       </c>
       <c r="G23">
         <f t="shared" si="7"/>
-        <v>74.217553</v>
+        <v>3.76246712</v>
       </c>
       <c r="H23">
         <f t="shared" si="8"/>
-        <v>74.21081575</v>
+        <v>3.627141965</v>
       </c>
       <c r="I23">
         <f t="shared" si="1"/>
-        <v>69.21071327</v>
+        <v>1.627067129</v>
       </c>
       <c r="J23">
         <f t="shared" si="2"/>
@@ -6641,7 +6656,7 @@
       </c>
       <c r="K23">
         <f t="shared" si="3"/>
-        <v>0.0001024765636</v>
+        <v>0.00007483570263</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="9"/>
@@ -6649,7 +6664,7 @@
       </c>
       <c r="N23">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -6670,27 +6685,27 @@
       </c>
       <c r="F24" s="3">
         <f t="shared" si="6"/>
-        <v>5.000017864</v>
+        <v>1.999990223</v>
       </c>
       <c r="G24">
         <f t="shared" si="7"/>
-        <v>74.21127409</v>
+        <v>3.762160231</v>
       </c>
       <c r="H24">
         <f t="shared" si="8"/>
-        <v>74.20453627</v>
+        <v>3.626823625</v>
       </c>
       <c r="I24">
         <f t="shared" si="1"/>
-        <v>69.2045184</v>
+        <v>1.626833402</v>
       </c>
       <c r="J24">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K24">
         <f t="shared" si="3"/>
-        <v>0.00001786387071</v>
+        <v>-0.000009776990305</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="9"/>
@@ -6698,7 +6713,7 @@
       </c>
       <c r="N24">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -6719,27 +6734,27 @@
       </c>
       <c r="F25" s="3">
         <f t="shared" si="6"/>
-        <v>4.999975558</v>
+        <v>2.000032529</v>
       </c>
       <c r="G25">
         <f t="shared" si="7"/>
-        <v>74.20813484</v>
+        <v>3.762313673</v>
       </c>
       <c r="H25">
         <f t="shared" si="8"/>
-        <v>74.20139673</v>
+        <v>3.626982792</v>
       </c>
       <c r="I25">
         <f t="shared" si="1"/>
-        <v>69.20142117</v>
+        <v>1.626950262</v>
       </c>
       <c r="J25">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K25">
         <f t="shared" si="3"/>
-        <v>-0.00002444247576</v>
+        <v>0.00003252935617</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="9"/>
@@ -6747,7 +6762,7 @@
       </c>
       <c r="N25">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
@@ -6768,27 +6783,27 @@
       </c>
       <c r="F26" s="3">
         <f t="shared" si="6"/>
-        <v>4.999996711</v>
+        <v>2.000011376</v>
       </c>
       <c r="G26">
         <f t="shared" si="7"/>
-        <v>74.20970445</v>
+        <v>3.762236951</v>
       </c>
       <c r="H26">
         <f t="shared" si="8"/>
-        <v>74.20296648</v>
+        <v>3.626903208</v>
       </c>
       <c r="I26">
         <f t="shared" si="1"/>
-        <v>69.20296977</v>
+        <v>1.626891831</v>
       </c>
       <c r="J26">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K26">
         <f t="shared" si="3"/>
-        <v>-0.000003289302526</v>
+        <v>0.00001137618293</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="9"/>
@@ -6796,7 +6811,7 @@
       </c>
       <c r="N26">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -6817,19 +6832,19 @@
       </c>
       <c r="F27" s="3">
         <f t="shared" si="6"/>
-        <v>5.000007287</v>
+        <v>2.0000008</v>
       </c>
       <c r="G27">
         <f t="shared" si="7"/>
-        <v>74.21048927</v>
+        <v>3.762198591</v>
       </c>
       <c r="H27">
         <f t="shared" si="8"/>
-        <v>74.20375137</v>
+        <v>3.626863416</v>
       </c>
       <c r="I27">
         <f t="shared" si="1"/>
-        <v>69.20374408</v>
+        <v>1.626862616</v>
       </c>
       <c r="J27">
         <f t="shared" si="2"/>
@@ -6837,7 +6852,7 @@
       </c>
       <c r="K27">
         <f t="shared" si="3"/>
-        <v>0.000007287284091</v>
+        <v>0.0000007995963127</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="9"/>
@@ -6845,7 +6860,7 @@
       </c>
       <c r="N27">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -6866,27 +6881,27 @@
       </c>
       <c r="F28" s="3">
         <f t="shared" si="6"/>
-        <v>5.000001999</v>
+        <v>1.999995511</v>
       </c>
       <c r="G28">
         <f t="shared" si="7"/>
-        <v>74.21009686</v>
+        <v>3.762179411</v>
       </c>
       <c r="H28">
         <f t="shared" si="8"/>
-        <v>74.20335892</v>
+        <v>3.626843521</v>
       </c>
       <c r="I28">
         <f t="shared" si="1"/>
-        <v>69.20335692</v>
+        <v>1.626848009</v>
       </c>
       <c r="J28">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K28">
         <f t="shared" si="3"/>
-        <v>0.000001998990782</v>
+        <v>-0.000004488696996</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="9"/>
@@ -6894,7 +6909,7 @@
       </c>
       <c r="N28">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -6915,19 +6930,19 @@
       </c>
       <c r="F29" s="3">
         <f t="shared" si="6"/>
-        <v>4.999999355</v>
+        <v>1.999998155</v>
       </c>
       <c r="G29">
         <f t="shared" si="7"/>
-        <v>74.20990065</v>
+        <v>3.762189001</v>
       </c>
       <c r="H29">
         <f t="shared" si="8"/>
-        <v>74.2031627</v>
+        <v>3.626853468</v>
       </c>
       <c r="I29">
         <f t="shared" si="1"/>
-        <v>69.20316335</v>
+        <v>1.626855313</v>
       </c>
       <c r="J29">
         <f t="shared" si="2"/>
@@ -6935,7 +6950,7 @@
       </c>
       <c r="K29">
         <f t="shared" si="3"/>
-        <v>-0.0000006451558727</v>
+        <v>-0.000001844550342</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="9"/>
@@ -6943,7 +6958,7 @@
       </c>
       <c r="N29">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -6964,27 +6979,27 @@
       </c>
       <c r="F30" s="3">
         <f t="shared" si="6"/>
-        <v>5.000000677</v>
+        <v>1.999999478</v>
       </c>
       <c r="G30">
         <f t="shared" si="7"/>
-        <v>74.20999875</v>
+        <v>3.762193796</v>
       </c>
       <c r="H30">
         <f t="shared" si="8"/>
-        <v>74.20326081</v>
+        <v>3.626858442</v>
       </c>
       <c r="I30">
         <f t="shared" si="1"/>
-        <v>69.20326013</v>
+        <v>1.626858965</v>
       </c>
       <c r="J30">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K30">
         <f t="shared" si="3"/>
-        <v>0.0000006769174545</v>
+        <v>-0.0000005224770145</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="9"/>
@@ -6992,7 +7007,7 @@
       </c>
       <c r="N30">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -7013,19 +7028,19 @@
       </c>
       <c r="F31" s="3">
         <f t="shared" si="6"/>
-        <v>5.000000016</v>
+        <v>2.000000139</v>
       </c>
       <c r="G31">
         <f t="shared" si="7"/>
-        <v>74.2099497</v>
+        <v>3.762196194</v>
       </c>
       <c r="H31">
         <f t="shared" si="8"/>
-        <v>74.20321176</v>
+        <v>3.626860929</v>
       </c>
       <c r="I31">
         <f t="shared" si="1"/>
-        <v>69.20321174</v>
+        <v>1.626860791</v>
       </c>
       <c r="J31">
         <f t="shared" si="2"/>
@@ -7033,7 +7048,7 @@
       </c>
       <c r="K31">
         <f t="shared" si="3"/>
-        <v>0.0000000158807909</v>
+        <v>0.0000001385596491</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" si="9"/>
@@ -7041,7 +7056,7 @@
       </c>
       <c r="N31">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -7062,19 +7077,19 @@
       </c>
       <c r="F32" s="3">
         <f t="shared" si="6"/>
-        <v>4.999999685</v>
+        <v>1.999999808</v>
       </c>
       <c r="G32">
         <f t="shared" si="7"/>
-        <v>74.20992518</v>
+        <v>3.762194995</v>
       </c>
       <c r="H32">
         <f t="shared" si="8"/>
-        <v>74.20318723</v>
+        <v>3.626859686</v>
       </c>
       <c r="I32">
         <f t="shared" si="1"/>
-        <v>69.20318754</v>
+        <v>1.626859878</v>
       </c>
       <c r="J32">
         <f t="shared" si="2"/>
@@ -7082,7 +7097,7 @@
       </c>
       <c r="K32">
         <f t="shared" si="3"/>
-        <v>-0.0000003146375409</v>
+        <v>-0.0000001919586827</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" si="9"/>
@@ -7090,7 +7105,7 @@
       </c>
       <c r="N32">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -7111,19 +7126,19 @@
       </c>
       <c r="F33" s="3">
         <f t="shared" si="6"/>
-        <v>4.999999851</v>
+        <v>1.999999973</v>
       </c>
       <c r="G33">
         <f t="shared" si="7"/>
-        <v>74.20993744</v>
+        <v>3.762195594</v>
       </c>
       <c r="H33">
         <f t="shared" si="8"/>
-        <v>74.20319949</v>
+        <v>3.626860307</v>
       </c>
       <c r="I33">
         <f t="shared" si="1"/>
-        <v>69.20319964</v>
+        <v>1.626860334</v>
       </c>
       <c r="J33">
         <f t="shared" si="2"/>
@@ -7131,7 +7146,7 @@
       </c>
       <c r="K33">
         <f t="shared" si="3"/>
-        <v>-0.0000001493783754</v>
+        <v>-0.00000002669951682</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" si="9"/>
@@ -7139,7 +7154,7 @@
       </c>
       <c r="N33">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -7160,27 +7175,27 @@
       </c>
       <c r="F34" s="3">
         <f t="shared" si="6"/>
-        <v>4.999999933</v>
+        <v>2.000000056</v>
       </c>
       <c r="G34">
         <f t="shared" si="7"/>
-        <v>74.20994357</v>
+        <v>3.762195894</v>
       </c>
       <c r="H34">
         <f t="shared" si="8"/>
-        <v>74.20320562</v>
+        <v>3.626860618</v>
       </c>
       <c r="I34">
         <f t="shared" si="1"/>
-        <v>69.20320569</v>
+        <v>1.626860562</v>
       </c>
       <c r="J34">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K34">
         <f t="shared" si="3"/>
-        <v>-0.00000006674879227</v>
+        <v>0.00000005593006591</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" si="9"/>
@@ -7188,7 +7203,7 @@
       </c>
       <c r="N34">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -7209,27 +7224,27 @@
       </c>
       <c r="F35" s="3">
         <f t="shared" si="6"/>
-        <v>4.999999975</v>
+        <v>2.000000015</v>
       </c>
       <c r="G35">
         <f t="shared" si="7"/>
-        <v>74.20994664</v>
+        <v>3.762195744</v>
       </c>
       <c r="H35">
         <f t="shared" si="8"/>
-        <v>74.20320869</v>
+        <v>3.626860463</v>
       </c>
       <c r="I35">
         <f t="shared" si="1"/>
-        <v>69.20320872</v>
+        <v>1.626860448</v>
       </c>
       <c r="J35">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K35">
         <f t="shared" si="3"/>
-        <v>-0.00000002543400068</v>
+        <v>0.00000001461527432</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" si="9"/>
@@ -7237,7 +7252,7 @@
       </c>
       <c r="N35">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -7258,19 +7273,19 @@
       </c>
       <c r="F36" s="3">
         <f t="shared" si="6"/>
-        <v>4.999999995</v>
+        <v>1.999999994</v>
       </c>
       <c r="G36">
         <f t="shared" si="7"/>
-        <v>74.20994817</v>
+        <v>3.762195669</v>
       </c>
       <c r="H36">
         <f t="shared" si="8"/>
-        <v>74.20321022</v>
+        <v>3.626860385</v>
       </c>
       <c r="I36">
         <f t="shared" si="1"/>
-        <v>69.20321023</v>
+        <v>1.626860391</v>
       </c>
       <c r="J36">
         <f t="shared" si="2"/>
@@ -7278,7 +7293,7 @@
       </c>
       <c r="K36">
         <f t="shared" si="3"/>
-        <v>-0.000000004776604889</v>
+        <v>-0.00000000604212147</v>
       </c>
       <c r="M36" t="str">
         <f t="shared" si="9"/>
@@ -7286,7 +7301,7 @@
       </c>
       <c r="N36">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -7307,19 +7322,19 @@
       </c>
       <c r="F37" s="3">
         <f t="shared" si="6"/>
-        <v>5.000000006</v>
+        <v>2.000000004</v>
       </c>
       <c r="G37">
         <f t="shared" si="7"/>
-        <v>74.20994894</v>
+        <v>3.762195707</v>
       </c>
       <c r="H37">
         <f t="shared" si="8"/>
-        <v>74.20321099</v>
+        <v>3.626860424</v>
       </c>
       <c r="I37">
         <f t="shared" si="1"/>
-        <v>69.20321098</v>
+        <v>1.62686042</v>
       </c>
       <c r="J37">
         <f t="shared" si="2"/>
@@ -7327,7 +7342,7 @@
       </c>
       <c r="K37">
         <f t="shared" si="3"/>
-        <v>0.000000005552093008</v>
+        <v>0.000000004286576427</v>
       </c>
     </row>
     <row r="38">
@@ -7348,27 +7363,27 @@
       </c>
       <c r="F38" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>1.999999999</v>
       </c>
       <c r="G38">
         <f t="shared" si="7"/>
-        <v>74.20994855</v>
+        <v>3.762195688</v>
       </c>
       <c r="H38">
         <f t="shared" si="8"/>
-        <v>74.20321061</v>
+        <v>3.626860405</v>
       </c>
       <c r="I38">
         <f t="shared" si="1"/>
-        <v>69.20321061</v>
+        <v>1.626860405</v>
       </c>
       <c r="J38">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K38">
         <f t="shared" si="3"/>
-        <v>0.0000000003877440591</v>
+        <v>-0.0000000008777725213</v>
       </c>
     </row>
     <row r="39">
@@ -7389,27 +7404,27 @@
       </c>
       <c r="F39" s="3">
         <f t="shared" si="6"/>
-        <v>4.999999998</v>
+        <v>2.000000002</v>
       </c>
       <c r="G39">
         <f t="shared" si="7"/>
-        <v>74.20994836</v>
+        <v>3.762195697</v>
       </c>
       <c r="H39">
         <f t="shared" si="8"/>
-        <v>74.20321041</v>
+        <v>3.626860414</v>
       </c>
       <c r="I39">
         <f t="shared" si="1"/>
-        <v>69.20321042</v>
+        <v>1.626860413</v>
       </c>
       <c r="J39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K39">
         <f t="shared" si="3"/>
-        <v>-0.000000002194430415</v>
+        <v>0.000000001704401953</v>
       </c>
     </row>
     <row r="40">
@@ -7430,27 +7445,27 @@
       </c>
       <c r="F40" s="3">
         <f t="shared" si="6"/>
-        <v>4.999999999</v>
+        <v>2</v>
       </c>
       <c r="G40">
         <f t="shared" si="7"/>
-        <v>74.20994846</v>
+        <v>3.762195693</v>
       </c>
       <c r="H40">
         <f t="shared" si="8"/>
-        <v>74.20321051</v>
+        <v>3.626860409</v>
       </c>
       <c r="I40">
         <f t="shared" si="1"/>
-        <v>69.20321051</v>
+        <v>1.626860409</v>
       </c>
       <c r="J40">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K40">
         <f t="shared" si="3"/>
-        <v>-0.000000000903343178</v>
+        <v>0.0000000004133147158</v>
       </c>
     </row>
     <row r="41">
@@ -7471,19 +7486,19 @@
       </c>
       <c r="F41" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G41">
         <f t="shared" si="7"/>
-        <v>74.20994851</v>
+        <v>3.76219569</v>
       </c>
       <c r="H41">
         <f t="shared" si="8"/>
-        <v>74.20321056</v>
+        <v>3.626860407</v>
       </c>
       <c r="I41">
         <f t="shared" si="1"/>
-        <v>69.20321056</v>
+        <v>1.626860407</v>
       </c>
       <c r="J41">
         <f t="shared" si="2"/>
@@ -7491,7 +7506,7 @@
       </c>
       <c r="K41">
         <f t="shared" si="3"/>
-        <v>-0.0000000002578000036</v>
+        <v>-0.0000000002322289028</v>
       </c>
     </row>
     <row r="42">
@@ -7512,19 +7527,19 @@
       </c>
       <c r="F42" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G42">
         <f t="shared" si="7"/>
-        <v>74.20994853</v>
+        <v>3.762195691</v>
       </c>
       <c r="H42">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I42">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J42">
         <f t="shared" si="2"/>
@@ -7553,19 +7568,19 @@
       </c>
       <c r="F43" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G43">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H43">
         <f t="shared" si="8"/>
-        <v>74.20321057</v>
+        <v>3.626860408</v>
       </c>
       <c r="I43">
         <f t="shared" si="1"/>
-        <v>69.20321057</v>
+        <v>1.626860408</v>
       </c>
       <c r="J43">
         <f t="shared" si="2"/>
@@ -7594,23 +7609,23 @@
       </c>
       <c r="F44" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G44">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H44">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I44">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J44">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K44">
         <f t="shared" si="3"/>
@@ -7635,23 +7650,23 @@
       </c>
       <c r="F45" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G45">
         <f t="shared" si="7"/>
-        <v>74.20994853</v>
+        <v>3.762195691</v>
       </c>
       <c r="H45">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I45">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J45">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K45">
         <f t="shared" si="3"/>
@@ -7676,23 +7691,23 @@
       </c>
       <c r="F46" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G46">
         <f t="shared" si="7"/>
-        <v>74.20994853</v>
+        <v>3.762195691</v>
       </c>
       <c r="H46">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I46">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J46">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K46">
         <f t="shared" si="3"/>
@@ -7717,19 +7732,19 @@
       </c>
       <c r="F47" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G47">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H47">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I47">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J47">
         <f t="shared" si="2"/>
@@ -7758,23 +7773,23 @@
       </c>
       <c r="F48" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G48">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H48">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I48">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J48">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K48">
         <f t="shared" si="3"/>
@@ -7799,19 +7814,19 @@
       </c>
       <c r="F49" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G49">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H49">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I49">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J49">
         <f t="shared" si="2"/>
@@ -7840,19 +7855,19 @@
       </c>
       <c r="F50" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G50">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H50">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I50">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J50">
         <f t="shared" si="2"/>
@@ -7881,19 +7896,19 @@
       </c>
       <c r="F51" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G51">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H51">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I51">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J51">
         <f t="shared" si="2"/>
@@ -7922,23 +7937,23 @@
       </c>
       <c r="F52" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G52">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H52">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I52">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J52">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K52">
         <f t="shared" si="3"/>
@@ -7963,19 +7978,19 @@
       </c>
       <c r="F53" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G53">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H53">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I53">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J53">
         <f t="shared" si="2"/>
@@ -8004,23 +8019,23 @@
       </c>
       <c r="F54" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G54">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H54">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I54">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J54">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K54">
         <f t="shared" si="3"/>
@@ -8045,23 +8060,23 @@
       </c>
       <c r="F55" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G55">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H55">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I55">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J55">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K55">
         <f t="shared" si="3"/>
@@ -8086,19 +8101,19 @@
       </c>
       <c r="F56" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G56">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H56">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I56">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J56">
         <f t="shared" si="2"/>
@@ -8127,19 +8142,19 @@
       </c>
       <c r="F57" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G57">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H57">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I57">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J57">
         <f t="shared" si="2"/>
@@ -8168,19 +8183,19 @@
       </c>
       <c r="F58" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G58">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H58">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I58">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J58">
         <f t="shared" si="2"/>
@@ -8209,19 +8224,19 @@
       </c>
       <c r="F59" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G59">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H59">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I59">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J59">
         <f t="shared" si="2"/>
@@ -8250,23 +8265,23 @@
       </c>
       <c r="F60" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G60">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H60">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I60">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J60">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K60">
         <f t="shared" si="3"/>
@@ -8291,23 +8306,23 @@
       </c>
       <c r="F61" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G61">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H61">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I61">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J61">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K61">
         <f t="shared" si="3"/>
@@ -8332,19 +8347,19 @@
       </c>
       <c r="F62" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G62">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H62">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I62">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J62">
         <f t="shared" si="2"/>
@@ -8373,23 +8388,23 @@
       </c>
       <c r="F63" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G63">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H63">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I63">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J63">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K63">
         <f t="shared" si="3"/>
@@ -8414,19 +8429,19 @@
       </c>
       <c r="F64" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G64">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H64">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I64">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J64">
         <f t="shared" si="2"/>
@@ -8455,19 +8470,19 @@
       </c>
       <c r="F65" s="3">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G65">
         <f t="shared" si="7"/>
-        <v>74.20994852</v>
+        <v>3.762195691</v>
       </c>
       <c r="H65">
         <f t="shared" si="8"/>
-        <v>74.20321058</v>
+        <v>3.626860408</v>
       </c>
       <c r="I65">
         <f t="shared" si="1"/>
-        <v>69.20321058</v>
+        <v>1.626860408</v>
       </c>
       <c r="J65">
         <f t="shared" si="2"/>

</xml_diff>